<commit_message>
Small tweaks to new columns for permits needing review
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A882D8-0FA0-4ED7-B312-6A3BAF779753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C6561-CE89-4229-942F-6AF62FF1B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="Pin_Error" sheetId="1" r:id="rId2"/>
-    <sheet name="Other" sheetId="3" r:id="rId3"/>
+    <sheet name="PIN Errors" sheetId="1" r:id="rId2"/>
+    <sheet name="Other Errors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="93">
   <si>
     <t># [LLINE]</t>
   </si>
@@ -152,9 +152,6 @@
     <t>This workbook contains permits extracted from the City of Chicago Data Portal that we could not automatically clean for upload to Smartfile.</t>
   </si>
   <si>
-    <t>We could not clean these permits because they are missing columns that Smartfile requires.</t>
-  </si>
-  <si>
     <t>Here's what each column means:</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>Suggested PINs</t>
   </si>
   <si>
-    <t xml:space="preserve">The address of the property. Clicking the link takes you to the search result for the address in CookViewer. Only present when the PIN is flagged as missing or invalid. </t>
-  </si>
-  <si>
     <t>Our best guess as to possible PINs for the property. Clicking the link takes you to the PIN detail view on the Assessor website. Only present for missing/invalid PINs.</t>
   </si>
   <si>
@@ -278,20 +272,56 @@
     <t>"Yes" if the work description is missing. Empty otherwise.</t>
   </si>
   <si>
-    <t>Likely Assessable?</t>
-  </si>
-  <si>
     <t>"Yes" if the work description contains terms that indicate the permit is likely to be assessable. Empty otherwise.</t>
   </si>
   <si>
     <t>Likely Assessable</t>
+  </si>
+  <si>
+    <t>Column descriptions</t>
+  </si>
+  <si>
+    <t>The address of the property. Clicking the link takes you to the search result for the address in CookViewer.</t>
+  </si>
+  <si>
+    <t>Tab descriptions</t>
+  </si>
+  <si>
+    <t>We could not clean these permits because they are missing columns that Smartfile requires, or their columns contain values that violate the constraints that Smartfile imposes on uploads.</t>
+  </si>
+  <si>
+    <t>There are three tabs in this workbook:</t>
+  </si>
+  <si>
+    <t>Tab name</t>
+  </si>
+  <si>
+    <t>Tab description</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>[This tab] Instructions for how to use this workbook.</t>
+  </si>
+  <si>
+    <t>PIN Errors</t>
+  </si>
+  <si>
+    <t>Permit rows with missing or invalid PINs.</t>
+  </si>
+  <si>
+    <t>Other Errors</t>
+  </si>
+  <si>
+    <t>Permit rows with all other types of errors except for missing or invalid PINs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,8 +365,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,8 +398,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -385,14 +428,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -409,17 +460,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,9 +495,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,9 +535,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -514,26 +570,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,26 +605,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -759,11 +781,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDD913F-9030-4CD4-850D-F7EAF1DE7A4C}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -773,9 +793,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
+      <c r="B1" s="15"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -784,346 +805,393 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="13"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="12" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="12"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>81</v>
+    <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A53" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="15"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1131,562 +1199,562 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A623" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG632" sqref="AG632"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="16" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.85546875" style="12" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:38" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="18" t="s">
+      <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="18" t="s">
+      <c r="AI1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>82</v>
+      <c r="AK1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="17"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="17"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="17"/>
+      <c r="AJ8" s="19"/>
+      <c r="AK8" s="19"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="17"/>
-      <c r="AK9" s="17"/>
+      <c r="AJ9" s="19"/>
+      <c r="AK9" s="19"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="17"/>
-      <c r="AK10" s="17"/>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
+      <c r="AJ12" s="19"/>
+      <c r="AK12" s="19"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="17"/>
-      <c r="AK13" s="17"/>
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="17"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="17"/>
-      <c r="AK15" s="17"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="17"/>
-      <c r="AK16" s="17"/>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
     </row>
     <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="17"/>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
     </row>
     <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="17"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
     </row>
     <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="19"/>
     </row>
     <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="17"/>
-      <c r="AK20" s="17"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="19"/>
     </row>
     <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
     </row>
     <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="17"/>
-      <c r="AK22" s="17"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
     </row>
     <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="17"/>
-      <c r="AK23" s="17"/>
+      <c r="AJ23" s="19"/>
+      <c r="AK23" s="19"/>
     </row>
     <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="17"/>
-      <c r="AK24" s="17"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
     </row>
     <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="17"/>
-      <c r="AK25" s="17"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
     </row>
     <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="17"/>
-      <c r="AK26" s="17"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
     </row>
     <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
     </row>
     <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="17"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
     </row>
     <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="17"/>
-      <c r="AK29" s="17"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
     </row>
     <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
     </row>
     <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="17"/>
-      <c r="AK31" s="17"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="19"/>
     </row>
     <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
+      <c r="AJ32" s="19"/>
+      <c r="AK32" s="19"/>
     </row>
     <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="17"/>
-      <c r="AK33" s="17"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
     </row>
     <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="17"/>
-      <c r="AK34" s="17"/>
+      <c r="AJ34" s="19"/>
+      <c r="AK34" s="19"/>
     </row>
     <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
     </row>
     <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="17"/>
-      <c r="AK36" s="17"/>
+      <c r="AJ36" s="19"/>
+      <c r="AK36" s="19"/>
     </row>
     <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="17"/>
-      <c r="AK37" s="17"/>
+      <c r="AJ37" s="19"/>
+      <c r="AK37" s="19"/>
     </row>
     <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="17"/>
-      <c r="AK38" s="17"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
     </row>
     <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="17"/>
-      <c r="AK39" s="17"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
     </row>
     <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="17"/>
-      <c r="AK40" s="17"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
     </row>
     <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="17"/>
-      <c r="AK41" s="17"/>
+      <c r="AJ41" s="19"/>
+      <c r="AK41" s="19"/>
     </row>
     <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="17"/>
-      <c r="AK42" s="17"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
     </row>
     <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
     </row>
     <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="17"/>
-      <c r="AK44" s="17"/>
+      <c r="AJ44" s="19"/>
+      <c r="AK44" s="19"/>
     </row>
     <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17"/>
+      <c r="AJ45" s="19"/>
+      <c r="AK45" s="19"/>
     </row>
     <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
     </row>
     <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
+      <c r="AJ47" s="19"/>
+      <c r="AK47" s="19"/>
     </row>
     <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="17"/>
-      <c r="AK48" s="17"/>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
     </row>
     <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="17"/>
-      <c r="AK49" s="17"/>
+      <c r="AJ49" s="19"/>
+      <c r="AK49" s="19"/>
     </row>
     <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="17"/>
-      <c r="AK50" s="17"/>
+      <c r="AJ50" s="19"/>
+      <c r="AK50" s="19"/>
     </row>
     <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
+      <c r="AJ51" s="19"/>
+      <c r="AK51" s="19"/>
     </row>
     <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="17"/>
-      <c r="AK52" s="17"/>
+      <c r="AJ52" s="19"/>
+      <c r="AK52" s="19"/>
     </row>
     <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="17"/>
-      <c r="AK53" s="17"/>
+      <c r="AJ53" s="19"/>
+      <c r="AK53" s="19"/>
     </row>
     <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="17"/>
-      <c r="AK54" s="17"/>
+      <c r="AJ54" s="19"/>
+      <c r="AK54" s="19"/>
     </row>
     <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="17"/>
-      <c r="AK55" s="17"/>
+      <c r="AJ55" s="19"/>
+      <c r="AK55" s="19"/>
     </row>
     <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="17"/>
-      <c r="AK56" s="17"/>
+      <c r="AJ56" s="19"/>
+      <c r="AK56" s="19"/>
     </row>
     <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="17"/>
-      <c r="AK57" s="17"/>
+      <c r="AJ57" s="19"/>
+      <c r="AK57" s="19"/>
     </row>
     <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="17"/>
-      <c r="AK58" s="17"/>
+      <c r="AJ58" s="19"/>
+      <c r="AK58" s="19"/>
     </row>
     <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
+      <c r="AJ59" s="19"/>
+      <c r="AK59" s="19"/>
     </row>
     <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="17"/>
-      <c r="AK60" s="17"/>
+      <c r="AJ60" s="19"/>
+      <c r="AK60" s="19"/>
     </row>
     <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="17"/>
-      <c r="AK61" s="17"/>
+      <c r="AJ61" s="19"/>
+      <c r="AK61" s="19"/>
     </row>
     <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="17"/>
-      <c r="AK62" s="17"/>
+      <c r="AJ62" s="19"/>
+      <c r="AK62" s="19"/>
     </row>
     <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="17"/>
-      <c r="AK63" s="17"/>
+      <c r="AJ63" s="19"/>
+      <c r="AK63" s="19"/>
     </row>
     <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="17"/>
-      <c r="AK64" s="17"/>
+      <c r="AJ64" s="19"/>
+      <c r="AK64" s="19"/>
     </row>
     <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="17"/>
-      <c r="AK65" s="17"/>
+      <c r="AJ65" s="19"/>
+      <c r="AK65" s="19"/>
     </row>
     <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="17"/>
-      <c r="AK66" s="17"/>
+      <c r="AJ66" s="19"/>
+      <c r="AK66" s="19"/>
     </row>
     <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="17"/>
-      <c r="AK67" s="17"/>
+      <c r="AJ67" s="19"/>
+      <c r="AK67" s="19"/>
     </row>
     <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="17"/>
-      <c r="AK68" s="17"/>
+      <c r="AJ68" s="19"/>
+      <c r="AK68" s="19"/>
     </row>
     <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
+      <c r="AJ69" s="19"/>
+      <c r="AK69" s="19"/>
     </row>
     <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="17"/>
-      <c r="AK70" s="17"/>
+      <c r="AJ70" s="19"/>
+      <c r="AK70" s="19"/>
     </row>
     <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="17"/>
-      <c r="AK71" s="17"/>
+      <c r="AJ71" s="19"/>
+      <c r="AK71" s="19"/>
     </row>
     <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="17"/>
-      <c r="AK72" s="17"/>
+      <c r="AJ72" s="19"/>
+      <c r="AK72" s="19"/>
     </row>
     <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="17"/>
-      <c r="AK73" s="17"/>
+      <c r="AJ73" s="19"/>
+      <c r="AK73" s="19"/>
     </row>
     <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="17"/>
-      <c r="AK74" s="17"/>
+      <c r="AJ74" s="19"/>
+      <c r="AK74" s="19"/>
     </row>
     <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="17"/>
-      <c r="AK75" s="17"/>
+      <c r="AJ75" s="19"/>
+      <c r="AK75" s="19"/>
     </row>
     <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="17"/>
-      <c r="AK76" s="17"/>
+      <c r="AJ76" s="19"/>
+      <c r="AK76" s="19"/>
     </row>
     <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="17"/>
-      <c r="AK77" s="17"/>
+      <c r="AJ77" s="19"/>
+      <c r="AK77" s="19"/>
     </row>
     <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
+      <c r="AJ78" s="19"/>
+      <c r="AK78" s="19"/>
     </row>
     <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="17"/>
-      <c r="AK79" s="17"/>
+      <c r="AJ79" s="19"/>
+      <c r="AK79" s="19"/>
     </row>
     <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="17"/>
-      <c r="AK80" s="17"/>
+      <c r="AJ80" s="19"/>
+      <c r="AK80" s="19"/>
     </row>
     <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="17"/>
-      <c r="AK81" s="17"/>
+      <c r="AJ81" s="19"/>
+      <c r="AK81" s="19"/>
     </row>
     <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="17"/>
-      <c r="AK82" s="17"/>
+      <c r="AJ82" s="19"/>
+      <c r="AK82" s="19"/>
     </row>
     <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="17"/>
-      <c r="AK83" s="17"/>
+      <c r="AJ83" s="19"/>
+      <c r="AK83" s="19"/>
     </row>
     <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="17"/>
-      <c r="AK84" s="17"/>
+      <c r="AJ84" s="19"/>
+      <c r="AK84" s="19"/>
     </row>
     <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="17"/>
-      <c r="AK85" s="17"/>
+      <c r="AJ85" s="19"/>
+      <c r="AK85" s="19"/>
     </row>
     <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="17"/>
-      <c r="AK86" s="17"/>
+      <c r="AJ86" s="19"/>
+      <c r="AK86" s="19"/>
     </row>
     <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="17"/>
-      <c r="AK87" s="17"/>
+      <c r="AJ87" s="19"/>
+      <c r="AK87" s="19"/>
     </row>
     <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="17"/>
-      <c r="AK88" s="17"/>
+      <c r="AJ88" s="19"/>
+      <c r="AK88" s="19"/>
     </row>
     <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="17"/>
-      <c r="AK89" s="17"/>
+      <c r="AJ89" s="19"/>
+      <c r="AK89" s="19"/>
     </row>
     <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="17"/>
-      <c r="AK90" s="17"/>
+      <c r="AJ90" s="19"/>
+      <c r="AK90" s="19"/>
     </row>
     <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="17"/>
-      <c r="AK91" s="17"/>
+      <c r="AJ91" s="19"/>
+      <c r="AK91" s="19"/>
     </row>
     <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="17"/>
-      <c r="AK92" s="17"/>
+      <c r="AJ92" s="19"/>
+      <c r="AK92" s="19"/>
     </row>
     <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="17"/>
-      <c r="AK93" s="17"/>
+      <c r="AJ93" s="19"/>
+      <c r="AK93" s="19"/>
     </row>
     <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="17"/>
-      <c r="AK94" s="17"/>
+      <c r="AJ94" s="19"/>
+      <c r="AK94" s="19"/>
     </row>
     <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="17"/>
-      <c r="AK95" s="17"/>
+      <c r="AJ95" s="19"/>
+      <c r="AK95" s="19"/>
     </row>
     <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="17"/>
-      <c r="AK96" s="17"/>
+      <c r="AJ96" s="19"/>
+      <c r="AK96" s="19"/>
     </row>
     <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="17"/>
-      <c r="AK97" s="17"/>
+      <c r="AJ97" s="19"/>
+      <c r="AK97" s="19"/>
     </row>
     <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="17"/>
-      <c r="AK98" s="17"/>
+      <c r="AJ98" s="19"/>
+      <c r="AK98" s="19"/>
     </row>
     <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="17"/>
-      <c r="AK99" s="17"/>
+      <c r="AJ99" s="19"/>
+      <c r="AK99" s="19"/>
     </row>
     <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="17"/>
-      <c r="AK100" s="17"/>
+      <c r="AJ100" s="19"/>
+      <c r="AK100" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1698,561 +1766,562 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="16" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.7109375" style="12" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="18" t="s">
+      <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="18" t="s">
+      <c r="AI1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>82</v>
+      <c r="AK1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="17"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="17"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="17"/>
+      <c r="AJ8" s="19"/>
+      <c r="AK8" s="19"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="17"/>
-      <c r="AK9" s="17"/>
+      <c r="AJ9" s="19"/>
+      <c r="AK9" s="19"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="17"/>
-      <c r="AK10" s="17"/>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
+      <c r="AJ12" s="19"/>
+      <c r="AK12" s="19"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="17"/>
-      <c r="AK13" s="17"/>
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="17"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="17"/>
-      <c r="AK15" s="17"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="17"/>
-      <c r="AK16" s="17"/>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
     </row>
     <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="17"/>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
     </row>
     <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="17"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
     </row>
     <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="19"/>
     </row>
     <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="17"/>
-      <c r="AK20" s="17"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="19"/>
     </row>
     <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
     </row>
     <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="17"/>
-      <c r="AK22" s="17"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
     </row>
     <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="17"/>
-      <c r="AK23" s="17"/>
+      <c r="AJ23" s="19"/>
+      <c r="AK23" s="19"/>
     </row>
     <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="17"/>
-      <c r="AK24" s="17"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
     </row>
     <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="17"/>
-      <c r="AK25" s="17"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
     </row>
     <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="17"/>
-      <c r="AK26" s="17"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
     </row>
     <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
     </row>
     <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="17"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
     </row>
     <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="17"/>
-      <c r="AK29" s="17"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
     </row>
     <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
     </row>
     <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="17"/>
-      <c r="AK31" s="17"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="19"/>
     </row>
     <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
+      <c r="AJ32" s="19"/>
+      <c r="AK32" s="19"/>
     </row>
     <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="17"/>
-      <c r="AK33" s="17"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
     </row>
     <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="17"/>
-      <c r="AK34" s="17"/>
+      <c r="AJ34" s="19"/>
+      <c r="AK34" s="19"/>
     </row>
     <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
     </row>
     <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="17"/>
-      <c r="AK36" s="17"/>
+      <c r="AJ36" s="19"/>
+      <c r="AK36" s="19"/>
     </row>
     <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="17"/>
-      <c r="AK37" s="17"/>
+      <c r="AJ37" s="19"/>
+      <c r="AK37" s="19"/>
     </row>
     <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="17"/>
-      <c r="AK38" s="17"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
     </row>
     <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="17"/>
-      <c r="AK39" s="17"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
     </row>
     <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="17"/>
-      <c r="AK40" s="17"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
     </row>
     <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="17"/>
-      <c r="AK41" s="17"/>
+      <c r="AJ41" s="19"/>
+      <c r="AK41" s="19"/>
     </row>
     <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="17"/>
-      <c r="AK42" s="17"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
     </row>
     <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
     </row>
     <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="17"/>
-      <c r="AK44" s="17"/>
+      <c r="AJ44" s="19"/>
+      <c r="AK44" s="19"/>
     </row>
     <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17"/>
+      <c r="AJ45" s="19"/>
+      <c r="AK45" s="19"/>
     </row>
     <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
     </row>
     <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
+      <c r="AJ47" s="19"/>
+      <c r="AK47" s="19"/>
     </row>
     <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="17"/>
-      <c r="AK48" s="17"/>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
     </row>
     <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="17"/>
-      <c r="AK49" s="17"/>
+      <c r="AJ49" s="19"/>
+      <c r="AK49" s="19"/>
     </row>
     <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="17"/>
-      <c r="AK50" s="17"/>
+      <c r="AJ50" s="19"/>
+      <c r="AK50" s="19"/>
     </row>
     <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
+      <c r="AJ51" s="19"/>
+      <c r="AK51" s="19"/>
     </row>
     <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="17"/>
-      <c r="AK52" s="17"/>
+      <c r="AJ52" s="19"/>
+      <c r="AK52" s="19"/>
     </row>
     <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="17"/>
-      <c r="AK53" s="17"/>
+      <c r="AJ53" s="19"/>
+      <c r="AK53" s="19"/>
     </row>
     <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="17"/>
-      <c r="AK54" s="17"/>
+      <c r="AJ54" s="19"/>
+      <c r="AK54" s="19"/>
     </row>
     <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="17"/>
-      <c r="AK55" s="17"/>
+      <c r="AJ55" s="19"/>
+      <c r="AK55" s="19"/>
     </row>
     <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="17"/>
-      <c r="AK56" s="17"/>
+      <c r="AJ56" s="19"/>
+      <c r="AK56" s="19"/>
     </row>
     <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="17"/>
-      <c r="AK57" s="17"/>
+      <c r="AJ57" s="19"/>
+      <c r="AK57" s="19"/>
     </row>
     <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="17"/>
-      <c r="AK58" s="17"/>
+      <c r="AJ58" s="19"/>
+      <c r="AK58" s="19"/>
     </row>
     <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
+      <c r="AJ59" s="19"/>
+      <c r="AK59" s="19"/>
     </row>
     <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="17"/>
-      <c r="AK60" s="17"/>
+      <c r="AJ60" s="19"/>
+      <c r="AK60" s="19"/>
     </row>
     <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="17"/>
-      <c r="AK61" s="17"/>
+      <c r="AJ61" s="19"/>
+      <c r="AK61" s="19"/>
     </row>
     <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="17"/>
-      <c r="AK62" s="17"/>
+      <c r="AJ62" s="19"/>
+      <c r="AK62" s="19"/>
     </row>
     <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="17"/>
-      <c r="AK63" s="17"/>
+      <c r="AJ63" s="19"/>
+      <c r="AK63" s="19"/>
     </row>
     <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="17"/>
-      <c r="AK64" s="17"/>
+      <c r="AJ64" s="19"/>
+      <c r="AK64" s="19"/>
     </row>
     <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="17"/>
-      <c r="AK65" s="17"/>
+      <c r="AJ65" s="19"/>
+      <c r="AK65" s="19"/>
     </row>
     <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="17"/>
-      <c r="AK66" s="17"/>
+      <c r="AJ66" s="19"/>
+      <c r="AK66" s="19"/>
     </row>
     <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="17"/>
-      <c r="AK67" s="17"/>
+      <c r="AJ67" s="19"/>
+      <c r="AK67" s="19"/>
     </row>
     <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="17"/>
-      <c r="AK68" s="17"/>
+      <c r="AJ68" s="19"/>
+      <c r="AK68" s="19"/>
     </row>
     <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
+      <c r="AJ69" s="19"/>
+      <c r="AK69" s="19"/>
     </row>
     <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="17"/>
-      <c r="AK70" s="17"/>
+      <c r="AJ70" s="19"/>
+      <c r="AK70" s="19"/>
     </row>
     <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="17"/>
-      <c r="AK71" s="17"/>
+      <c r="AJ71" s="19"/>
+      <c r="AK71" s="19"/>
     </row>
     <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="17"/>
-      <c r="AK72" s="17"/>
+      <c r="AJ72" s="19"/>
+      <c r="AK72" s="19"/>
     </row>
     <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="17"/>
-      <c r="AK73" s="17"/>
+      <c r="AJ73" s="19"/>
+      <c r="AK73" s="19"/>
     </row>
     <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="17"/>
-      <c r="AK74" s="17"/>
+      <c r="AJ74" s="19"/>
+      <c r="AK74" s="19"/>
     </row>
     <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="17"/>
-      <c r="AK75" s="17"/>
+      <c r="AJ75" s="19"/>
+      <c r="AK75" s="19"/>
     </row>
     <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="17"/>
-      <c r="AK76" s="17"/>
+      <c r="AJ76" s="19"/>
+      <c r="AK76" s="19"/>
     </row>
     <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="17"/>
-      <c r="AK77" s="17"/>
+      <c r="AJ77" s="19"/>
+      <c r="AK77" s="19"/>
     </row>
     <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
+      <c r="AJ78" s="19"/>
+      <c r="AK78" s="19"/>
     </row>
     <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="17"/>
-      <c r="AK79" s="17"/>
+      <c r="AJ79" s="19"/>
+      <c r="AK79" s="19"/>
     </row>
     <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="17"/>
-      <c r="AK80" s="17"/>
+      <c r="AJ80" s="19"/>
+      <c r="AK80" s="19"/>
     </row>
     <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="17"/>
-      <c r="AK81" s="17"/>
+      <c r="AJ81" s="19"/>
+      <c r="AK81" s="19"/>
     </row>
     <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="17"/>
-      <c r="AK82" s="17"/>
+      <c r="AJ82" s="19"/>
+      <c r="AK82" s="19"/>
     </row>
     <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="17"/>
-      <c r="AK83" s="17"/>
+      <c r="AJ83" s="19"/>
+      <c r="AK83" s="19"/>
     </row>
     <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="17"/>
-      <c r="AK84" s="17"/>
+      <c r="AJ84" s="19"/>
+      <c r="AK84" s="19"/>
     </row>
     <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="17"/>
-      <c r="AK85" s="17"/>
+      <c r="AJ85" s="19"/>
+      <c r="AK85" s="19"/>
     </row>
     <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="17"/>
-      <c r="AK86" s="17"/>
+      <c r="AJ86" s="19"/>
+      <c r="AK86" s="19"/>
     </row>
     <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="17"/>
-      <c r="AK87" s="17"/>
+      <c r="AJ87" s="19"/>
+      <c r="AK87" s="19"/>
     </row>
     <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="17"/>
-      <c r="AK88" s="17"/>
+      <c r="AJ88" s="19"/>
+      <c r="AK88" s="19"/>
     </row>
     <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="17"/>
-      <c r="AK89" s="17"/>
+      <c r="AJ89" s="19"/>
+      <c r="AK89" s="19"/>
     </row>
     <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="17"/>
-      <c r="AK90" s="17"/>
+      <c r="AJ90" s="19"/>
+      <c r="AK90" s="19"/>
     </row>
     <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="17"/>
-      <c r="AK91" s="17"/>
+      <c r="AJ91" s="19"/>
+      <c r="AK91" s="19"/>
     </row>
     <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="17"/>
-      <c r="AK92" s="17"/>
+      <c r="AJ92" s="19"/>
+      <c r="AK92" s="19"/>
     </row>
     <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="17"/>
-      <c r="AK93" s="17"/>
+      <c r="AJ93" s="19"/>
+      <c r="AK93" s="19"/>
     </row>
     <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="17"/>
-      <c r="AK94" s="17"/>
+      <c r="AJ94" s="19"/>
+      <c r="AK94" s="19"/>
     </row>
     <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="17"/>
-      <c r="AK95" s="17"/>
+      <c r="AJ95" s="19"/>
+      <c r="AK95" s="19"/>
     </row>
     <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="17"/>
-      <c r="AK96" s="17"/>
+      <c r="AJ96" s="19"/>
+      <c r="AK96" s="19"/>
     </row>
     <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="17"/>
-      <c r="AK97" s="17"/>
+      <c r="AJ97" s="19"/>
+      <c r="AK97" s="19"/>
     </row>
     <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="17"/>
-      <c r="AK98" s="17"/>
+      <c r="AJ98" s="19"/>
+      <c r="AK98" s="19"/>
     </row>
     <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="17"/>
-      <c r="AK99" s="17"/>
+      <c r="AJ99" s="19"/>
+      <c r="AK99" s="19"/>
     </row>
     <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="17"/>
-      <c r="AK100" s="17"/>
+      <c r="AJ100" s="19"/>
+      <c r="AK100" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2260,26 +2329,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e9c3904391dfdb572e7cb9fb22afd49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9197d42b690c6e28e7629505631f20d" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -2514,10 +2563,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2534,20 +2614,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
-    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Small tweaks to new columns for permits needing review (#22)
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A882D8-0FA0-4ED7-B312-6A3BAF779753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C6561-CE89-4229-942F-6AF62FF1B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="Pin_Error" sheetId="1" r:id="rId2"/>
-    <sheet name="Other" sheetId="3" r:id="rId3"/>
+    <sheet name="PIN Errors" sheetId="1" r:id="rId2"/>
+    <sheet name="Other Errors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="93">
   <si>
     <t># [LLINE]</t>
   </si>
@@ -152,9 +152,6 @@
     <t>This workbook contains permits extracted from the City of Chicago Data Portal that we could not automatically clean for upload to Smartfile.</t>
   </si>
   <si>
-    <t>We could not clean these permits because they are missing columns that Smartfile requires.</t>
-  </si>
-  <si>
     <t>Here's what each column means:</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>Suggested PINs</t>
   </si>
   <si>
-    <t xml:space="preserve">The address of the property. Clicking the link takes you to the search result for the address in CookViewer. Only present when the PIN is flagged as missing or invalid. </t>
-  </si>
-  <si>
     <t>Our best guess as to possible PINs for the property. Clicking the link takes you to the PIN detail view on the Assessor website. Only present for missing/invalid PINs.</t>
   </si>
   <si>
@@ -278,20 +272,56 @@
     <t>"Yes" if the work description is missing. Empty otherwise.</t>
   </si>
   <si>
-    <t>Likely Assessable?</t>
-  </si>
-  <si>
     <t>"Yes" if the work description contains terms that indicate the permit is likely to be assessable. Empty otherwise.</t>
   </si>
   <si>
     <t>Likely Assessable</t>
+  </si>
+  <si>
+    <t>Column descriptions</t>
+  </si>
+  <si>
+    <t>The address of the property. Clicking the link takes you to the search result for the address in CookViewer.</t>
+  </si>
+  <si>
+    <t>Tab descriptions</t>
+  </si>
+  <si>
+    <t>We could not clean these permits because they are missing columns that Smartfile requires, or their columns contain values that violate the constraints that Smartfile imposes on uploads.</t>
+  </si>
+  <si>
+    <t>There are three tabs in this workbook:</t>
+  </si>
+  <si>
+    <t>Tab name</t>
+  </si>
+  <si>
+    <t>Tab description</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>[This tab] Instructions for how to use this workbook.</t>
+  </si>
+  <si>
+    <t>PIN Errors</t>
+  </si>
+  <si>
+    <t>Permit rows with missing or invalid PINs.</t>
+  </si>
+  <si>
+    <t>Other Errors</t>
+  </si>
+  <si>
+    <t>Permit rows with all other types of errors except for missing or invalid PINs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,8 +365,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,8 +398,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -385,14 +428,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -409,17 +460,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,9 +495,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,9 +535,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -514,26 +570,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,26 +605,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -759,11 +781,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDD913F-9030-4CD4-850D-F7EAF1DE7A4C}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -773,9 +793,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
+      <c r="B1" s="15"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -784,346 +805,393 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="13"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="12" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="12"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>81</v>
+    <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A53" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="15"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1131,562 +1199,562 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A623" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG632" sqref="AG632"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="16" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.85546875" style="12" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:38" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="18" t="s">
+      <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="18" t="s">
+      <c r="AI1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>82</v>
+      <c r="AK1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="17"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="17"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="17"/>
+      <c r="AJ8" s="19"/>
+      <c r="AK8" s="19"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="17"/>
-      <c r="AK9" s="17"/>
+      <c r="AJ9" s="19"/>
+      <c r="AK9" s="19"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="17"/>
-      <c r="AK10" s="17"/>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
+      <c r="AJ12" s="19"/>
+      <c r="AK12" s="19"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="17"/>
-      <c r="AK13" s="17"/>
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="17"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="17"/>
-      <c r="AK15" s="17"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="17"/>
-      <c r="AK16" s="17"/>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
     </row>
     <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="17"/>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
     </row>
     <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="17"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
     </row>
     <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="19"/>
     </row>
     <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="17"/>
-      <c r="AK20" s="17"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="19"/>
     </row>
     <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
     </row>
     <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="17"/>
-      <c r="AK22" s="17"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
     </row>
     <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="17"/>
-      <c r="AK23" s="17"/>
+      <c r="AJ23" s="19"/>
+      <c r="AK23" s="19"/>
     </row>
     <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="17"/>
-      <c r="AK24" s="17"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
     </row>
     <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="17"/>
-      <c r="AK25" s="17"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
     </row>
     <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="17"/>
-      <c r="AK26" s="17"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
     </row>
     <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
     </row>
     <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="17"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
     </row>
     <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="17"/>
-      <c r="AK29" s="17"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
     </row>
     <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
     </row>
     <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="17"/>
-      <c r="AK31" s="17"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="19"/>
     </row>
     <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
+      <c r="AJ32" s="19"/>
+      <c r="AK32" s="19"/>
     </row>
     <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="17"/>
-      <c r="AK33" s="17"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
     </row>
     <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="17"/>
-      <c r="AK34" s="17"/>
+      <c r="AJ34" s="19"/>
+      <c r="AK34" s="19"/>
     </row>
     <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
     </row>
     <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="17"/>
-      <c r="AK36" s="17"/>
+      <c r="AJ36" s="19"/>
+      <c r="AK36" s="19"/>
     </row>
     <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="17"/>
-      <c r="AK37" s="17"/>
+      <c r="AJ37" s="19"/>
+      <c r="AK37" s="19"/>
     </row>
     <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="17"/>
-      <c r="AK38" s="17"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
     </row>
     <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="17"/>
-      <c r="AK39" s="17"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
     </row>
     <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="17"/>
-      <c r="AK40" s="17"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
     </row>
     <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="17"/>
-      <c r="AK41" s="17"/>
+      <c r="AJ41" s="19"/>
+      <c r="AK41" s="19"/>
     </row>
     <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="17"/>
-      <c r="AK42" s="17"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
     </row>
     <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
     </row>
     <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="17"/>
-      <c r="AK44" s="17"/>
+      <c r="AJ44" s="19"/>
+      <c r="AK44" s="19"/>
     </row>
     <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17"/>
+      <c r="AJ45" s="19"/>
+      <c r="AK45" s="19"/>
     </row>
     <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
     </row>
     <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
+      <c r="AJ47" s="19"/>
+      <c r="AK47" s="19"/>
     </row>
     <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="17"/>
-      <c r="AK48" s="17"/>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
     </row>
     <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="17"/>
-      <c r="AK49" s="17"/>
+      <c r="AJ49" s="19"/>
+      <c r="AK49" s="19"/>
     </row>
     <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="17"/>
-      <c r="AK50" s="17"/>
+      <c r="AJ50" s="19"/>
+      <c r="AK50" s="19"/>
     </row>
     <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
+      <c r="AJ51" s="19"/>
+      <c r="AK51" s="19"/>
     </row>
     <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="17"/>
-      <c r="AK52" s="17"/>
+      <c r="AJ52" s="19"/>
+      <c r="AK52" s="19"/>
     </row>
     <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="17"/>
-      <c r="AK53" s="17"/>
+      <c r="AJ53" s="19"/>
+      <c r="AK53" s="19"/>
     </row>
     <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="17"/>
-      <c r="AK54" s="17"/>
+      <c r="AJ54" s="19"/>
+      <c r="AK54" s="19"/>
     </row>
     <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="17"/>
-      <c r="AK55" s="17"/>
+      <c r="AJ55" s="19"/>
+      <c r="AK55" s="19"/>
     </row>
     <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="17"/>
-      <c r="AK56" s="17"/>
+      <c r="AJ56" s="19"/>
+      <c r="AK56" s="19"/>
     </row>
     <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="17"/>
-      <c r="AK57" s="17"/>
+      <c r="AJ57" s="19"/>
+      <c r="AK57" s="19"/>
     </row>
     <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="17"/>
-      <c r="AK58" s="17"/>
+      <c r="AJ58" s="19"/>
+      <c r="AK58" s="19"/>
     </row>
     <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
+      <c r="AJ59" s="19"/>
+      <c r="AK59" s="19"/>
     </row>
     <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="17"/>
-      <c r="AK60" s="17"/>
+      <c r="AJ60" s="19"/>
+      <c r="AK60" s="19"/>
     </row>
     <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="17"/>
-      <c r="AK61" s="17"/>
+      <c r="AJ61" s="19"/>
+      <c r="AK61" s="19"/>
     </row>
     <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="17"/>
-      <c r="AK62" s="17"/>
+      <c r="AJ62" s="19"/>
+      <c r="AK62" s="19"/>
     </row>
     <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="17"/>
-      <c r="AK63" s="17"/>
+      <c r="AJ63" s="19"/>
+      <c r="AK63" s="19"/>
     </row>
     <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="17"/>
-      <c r="AK64" s="17"/>
+      <c r="AJ64" s="19"/>
+      <c r="AK64" s="19"/>
     </row>
     <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="17"/>
-      <c r="AK65" s="17"/>
+      <c r="AJ65" s="19"/>
+      <c r="AK65" s="19"/>
     </row>
     <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="17"/>
-      <c r="AK66" s="17"/>
+      <c r="AJ66" s="19"/>
+      <c r="AK66" s="19"/>
     </row>
     <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="17"/>
-      <c r="AK67" s="17"/>
+      <c r="AJ67" s="19"/>
+      <c r="AK67" s="19"/>
     </row>
     <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="17"/>
-      <c r="AK68" s="17"/>
+      <c r="AJ68" s="19"/>
+      <c r="AK68" s="19"/>
     </row>
     <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
+      <c r="AJ69" s="19"/>
+      <c r="AK69" s="19"/>
     </row>
     <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="17"/>
-      <c r="AK70" s="17"/>
+      <c r="AJ70" s="19"/>
+      <c r="AK70" s="19"/>
     </row>
     <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="17"/>
-      <c r="AK71" s="17"/>
+      <c r="AJ71" s="19"/>
+      <c r="AK71" s="19"/>
     </row>
     <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="17"/>
-      <c r="AK72" s="17"/>
+      <c r="AJ72" s="19"/>
+      <c r="AK72" s="19"/>
     </row>
     <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="17"/>
-      <c r="AK73" s="17"/>
+      <c r="AJ73" s="19"/>
+      <c r="AK73" s="19"/>
     </row>
     <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="17"/>
-      <c r="AK74" s="17"/>
+      <c r="AJ74" s="19"/>
+      <c r="AK74" s="19"/>
     </row>
     <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="17"/>
-      <c r="AK75" s="17"/>
+      <c r="AJ75" s="19"/>
+      <c r="AK75" s="19"/>
     </row>
     <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="17"/>
-      <c r="AK76" s="17"/>
+      <c r="AJ76" s="19"/>
+      <c r="AK76" s="19"/>
     </row>
     <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="17"/>
-      <c r="AK77" s="17"/>
+      <c r="AJ77" s="19"/>
+      <c r="AK77" s="19"/>
     </row>
     <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
+      <c r="AJ78" s="19"/>
+      <c r="AK78" s="19"/>
     </row>
     <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="17"/>
-      <c r="AK79" s="17"/>
+      <c r="AJ79" s="19"/>
+      <c r="AK79" s="19"/>
     </row>
     <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="17"/>
-      <c r="AK80" s="17"/>
+      <c r="AJ80" s="19"/>
+      <c r="AK80" s="19"/>
     </row>
     <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="17"/>
-      <c r="AK81" s="17"/>
+      <c r="AJ81" s="19"/>
+      <c r="AK81" s="19"/>
     </row>
     <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="17"/>
-      <c r="AK82" s="17"/>
+      <c r="AJ82" s="19"/>
+      <c r="AK82" s="19"/>
     </row>
     <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="17"/>
-      <c r="AK83" s="17"/>
+      <c r="AJ83" s="19"/>
+      <c r="AK83" s="19"/>
     </row>
     <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="17"/>
-      <c r="AK84" s="17"/>
+      <c r="AJ84" s="19"/>
+      <c r="AK84" s="19"/>
     </row>
     <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="17"/>
-      <c r="AK85" s="17"/>
+      <c r="AJ85" s="19"/>
+      <c r="AK85" s="19"/>
     </row>
     <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="17"/>
-      <c r="AK86" s="17"/>
+      <c r="AJ86" s="19"/>
+      <c r="AK86" s="19"/>
     </row>
     <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="17"/>
-      <c r="AK87" s="17"/>
+      <c r="AJ87" s="19"/>
+      <c r="AK87" s="19"/>
     </row>
     <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="17"/>
-      <c r="AK88" s="17"/>
+      <c r="AJ88" s="19"/>
+      <c r="AK88" s="19"/>
     </row>
     <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="17"/>
-      <c r="AK89" s="17"/>
+      <c r="AJ89" s="19"/>
+      <c r="AK89" s="19"/>
     </row>
     <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="17"/>
-      <c r="AK90" s="17"/>
+      <c r="AJ90" s="19"/>
+      <c r="AK90" s="19"/>
     </row>
     <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="17"/>
-      <c r="AK91" s="17"/>
+      <c r="AJ91" s="19"/>
+      <c r="AK91" s="19"/>
     </row>
     <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="17"/>
-      <c r="AK92" s="17"/>
+      <c r="AJ92" s="19"/>
+      <c r="AK92" s="19"/>
     </row>
     <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="17"/>
-      <c r="AK93" s="17"/>
+      <c r="AJ93" s="19"/>
+      <c r="AK93" s="19"/>
     </row>
     <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="17"/>
-      <c r="AK94" s="17"/>
+      <c r="AJ94" s="19"/>
+      <c r="AK94" s="19"/>
     </row>
     <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="17"/>
-      <c r="AK95" s="17"/>
+      <c r="AJ95" s="19"/>
+      <c r="AK95" s="19"/>
     </row>
     <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="17"/>
-      <c r="AK96" s="17"/>
+      <c r="AJ96" s="19"/>
+      <c r="AK96" s="19"/>
     </row>
     <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="17"/>
-      <c r="AK97" s="17"/>
+      <c r="AJ97" s="19"/>
+      <c r="AK97" s="19"/>
     </row>
     <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="17"/>
-      <c r="AK98" s="17"/>
+      <c r="AJ98" s="19"/>
+      <c r="AK98" s="19"/>
     </row>
     <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="17"/>
-      <c r="AK99" s="17"/>
+      <c r="AJ99" s="19"/>
+      <c r="AK99" s="19"/>
     </row>
     <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="17"/>
-      <c r="AK100" s="17"/>
+      <c r="AJ100" s="19"/>
+      <c r="AK100" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1698,561 +1766,562 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AL10" sqref="AL10"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="28" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="16" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.7109375" style="12" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
+    <col min="38" max="38" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="18" t="s">
+      <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="18" t="s">
+      <c r="AI1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL1" s="9" t="s">
-        <v>82</v>
+      <c r="AK1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="17"/>
-      <c r="AK2" s="17"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="17"/>
-      <c r="AK4" s="17"/>
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="17"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="19"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="17"/>
+      <c r="AJ7" s="19"/>
+      <c r="AK7" s="19"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="17"/>
+      <c r="AJ8" s="19"/>
+      <c r="AK8" s="19"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="17"/>
-      <c r="AK9" s="17"/>
+      <c r="AJ9" s="19"/>
+      <c r="AK9" s="19"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="17"/>
-      <c r="AK10" s="17"/>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="17"/>
-      <c r="AK12" s="17"/>
+      <c r="AJ12" s="19"/>
+      <c r="AK12" s="19"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="17"/>
-      <c r="AK13" s="17"/>
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="17"/>
-      <c r="AK14" s="17"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="17"/>
-      <c r="AK15" s="17"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="17"/>
-      <c r="AK16" s="17"/>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
     </row>
     <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="17"/>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
     </row>
     <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="17"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
     </row>
     <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="17"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="19"/>
     </row>
     <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="17"/>
-      <c r="AK20" s="17"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="19"/>
     </row>
     <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="17"/>
-      <c r="AK21" s="17"/>
+      <c r="AJ21" s="19"/>
+      <c r="AK21" s="19"/>
     </row>
     <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="17"/>
-      <c r="AK22" s="17"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
     </row>
     <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="17"/>
-      <c r="AK23" s="17"/>
+      <c r="AJ23" s="19"/>
+      <c r="AK23" s="19"/>
     </row>
     <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="17"/>
-      <c r="AK24" s="17"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
     </row>
     <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="17"/>
-      <c r="AK25" s="17"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
     </row>
     <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="17"/>
-      <c r="AK26" s="17"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
     </row>
     <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="17"/>
+      <c r="AJ27" s="19"/>
+      <c r="AK27" s="19"/>
     </row>
     <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="17"/>
-      <c r="AK28" s="17"/>
+      <c r="AJ28" s="19"/>
+      <c r="AK28" s="19"/>
     </row>
     <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="17"/>
-      <c r="AK29" s="17"/>
+      <c r="AJ29" s="19"/>
+      <c r="AK29" s="19"/>
     </row>
     <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="17"/>
+      <c r="AJ30" s="19"/>
+      <c r="AK30" s="19"/>
     </row>
     <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="17"/>
-      <c r="AK31" s="17"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="19"/>
     </row>
     <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
+      <c r="AJ32" s="19"/>
+      <c r="AK32" s="19"/>
     </row>
     <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="17"/>
-      <c r="AK33" s="17"/>
+      <c r="AJ33" s="19"/>
+      <c r="AK33" s="19"/>
     </row>
     <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="17"/>
-      <c r="AK34" s="17"/>
+      <c r="AJ34" s="19"/>
+      <c r="AK34" s="19"/>
     </row>
     <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
+      <c r="AJ35" s="19"/>
+      <c r="AK35" s="19"/>
     </row>
     <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="17"/>
-      <c r="AK36" s="17"/>
+      <c r="AJ36" s="19"/>
+      <c r="AK36" s="19"/>
     </row>
     <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="17"/>
-      <c r="AK37" s="17"/>
+      <c r="AJ37" s="19"/>
+      <c r="AK37" s="19"/>
     </row>
     <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="17"/>
-      <c r="AK38" s="17"/>
+      <c r="AJ38" s="19"/>
+      <c r="AK38" s="19"/>
     </row>
     <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="17"/>
-      <c r="AK39" s="17"/>
+      <c r="AJ39" s="19"/>
+      <c r="AK39" s="19"/>
     </row>
     <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="17"/>
-      <c r="AK40" s="17"/>
+      <c r="AJ40" s="19"/>
+      <c r="AK40" s="19"/>
     </row>
     <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="17"/>
-      <c r="AK41" s="17"/>
+      <c r="AJ41" s="19"/>
+      <c r="AK41" s="19"/>
     </row>
     <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="17"/>
-      <c r="AK42" s="17"/>
+      <c r="AJ42" s="19"/>
+      <c r="AK42" s="19"/>
     </row>
     <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="17"/>
-      <c r="AK43" s="17"/>
+      <c r="AJ43" s="19"/>
+      <c r="AK43" s="19"/>
     </row>
     <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="17"/>
-      <c r="AK44" s="17"/>
+      <c r="AJ44" s="19"/>
+      <c r="AK44" s="19"/>
     </row>
     <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="17"/>
+      <c r="AJ45" s="19"/>
+      <c r="AK45" s="19"/>
     </row>
     <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="17"/>
-      <c r="AK46" s="17"/>
+      <c r="AJ46" s="19"/>
+      <c r="AK46" s="19"/>
     </row>
     <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="17"/>
-      <c r="AK47" s="17"/>
+      <c r="AJ47" s="19"/>
+      <c r="AK47" s="19"/>
     </row>
     <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="17"/>
-      <c r="AK48" s="17"/>
+      <c r="AJ48" s="19"/>
+      <c r="AK48" s="19"/>
     </row>
     <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="17"/>
-      <c r="AK49" s="17"/>
+      <c r="AJ49" s="19"/>
+      <c r="AK49" s="19"/>
     </row>
     <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="17"/>
-      <c r="AK50" s="17"/>
+      <c r="AJ50" s="19"/>
+      <c r="AK50" s="19"/>
     </row>
     <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="17"/>
-      <c r="AK51" s="17"/>
+      <c r="AJ51" s="19"/>
+      <c r="AK51" s="19"/>
     </row>
     <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="17"/>
-      <c r="AK52" s="17"/>
+      <c r="AJ52" s="19"/>
+      <c r="AK52" s="19"/>
     </row>
     <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="17"/>
-      <c r="AK53" s="17"/>
+      <c r="AJ53" s="19"/>
+      <c r="AK53" s="19"/>
     </row>
     <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="17"/>
-      <c r="AK54" s="17"/>
+      <c r="AJ54" s="19"/>
+      <c r="AK54" s="19"/>
     </row>
     <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="17"/>
-      <c r="AK55" s="17"/>
+      <c r="AJ55" s="19"/>
+      <c r="AK55" s="19"/>
     </row>
     <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="17"/>
-      <c r="AK56" s="17"/>
+      <c r="AJ56" s="19"/>
+      <c r="AK56" s="19"/>
     </row>
     <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="17"/>
-      <c r="AK57" s="17"/>
+      <c r="AJ57" s="19"/>
+      <c r="AK57" s="19"/>
     </row>
     <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="17"/>
-      <c r="AK58" s="17"/>
+      <c r="AJ58" s="19"/>
+      <c r="AK58" s="19"/>
     </row>
     <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="17"/>
-      <c r="AK59" s="17"/>
+      <c r="AJ59" s="19"/>
+      <c r="AK59" s="19"/>
     </row>
     <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="17"/>
-      <c r="AK60" s="17"/>
+      <c r="AJ60" s="19"/>
+      <c r="AK60" s="19"/>
     </row>
     <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="17"/>
-      <c r="AK61" s="17"/>
+      <c r="AJ61" s="19"/>
+      <c r="AK61" s="19"/>
     </row>
     <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="17"/>
-      <c r="AK62" s="17"/>
+      <c r="AJ62" s="19"/>
+      <c r="AK62" s="19"/>
     </row>
     <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="17"/>
-      <c r="AK63" s="17"/>
+      <c r="AJ63" s="19"/>
+      <c r="AK63" s="19"/>
     </row>
     <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="17"/>
-      <c r="AK64" s="17"/>
+      <c r="AJ64" s="19"/>
+      <c r="AK64" s="19"/>
     </row>
     <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="17"/>
-      <c r="AK65" s="17"/>
+      <c r="AJ65" s="19"/>
+      <c r="AK65" s="19"/>
     </row>
     <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="17"/>
-      <c r="AK66" s="17"/>
+      <c r="AJ66" s="19"/>
+      <c r="AK66" s="19"/>
     </row>
     <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="17"/>
-      <c r="AK67" s="17"/>
+      <c r="AJ67" s="19"/>
+      <c r="AK67" s="19"/>
     </row>
     <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="17"/>
-      <c r="AK68" s="17"/>
+      <c r="AJ68" s="19"/>
+      <c r="AK68" s="19"/>
     </row>
     <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="17"/>
-      <c r="AK69" s="17"/>
+      <c r="AJ69" s="19"/>
+      <c r="AK69" s="19"/>
     </row>
     <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="17"/>
-      <c r="AK70" s="17"/>
+      <c r="AJ70" s="19"/>
+      <c r="AK70" s="19"/>
     </row>
     <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="17"/>
-      <c r="AK71" s="17"/>
+      <c r="AJ71" s="19"/>
+      <c r="AK71" s="19"/>
     </row>
     <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="17"/>
-      <c r="AK72" s="17"/>
+      <c r="AJ72" s="19"/>
+      <c r="AK72" s="19"/>
     </row>
     <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="17"/>
-      <c r="AK73" s="17"/>
+      <c r="AJ73" s="19"/>
+      <c r="AK73" s="19"/>
     </row>
     <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="17"/>
-      <c r="AK74" s="17"/>
+      <c r="AJ74" s="19"/>
+      <c r="AK74" s="19"/>
     </row>
     <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="17"/>
-      <c r="AK75" s="17"/>
+      <c r="AJ75" s="19"/>
+      <c r="AK75" s="19"/>
     </row>
     <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="17"/>
-      <c r="AK76" s="17"/>
+      <c r="AJ76" s="19"/>
+      <c r="AK76" s="19"/>
     </row>
     <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="17"/>
-      <c r="AK77" s="17"/>
+      <c r="AJ77" s="19"/>
+      <c r="AK77" s="19"/>
     </row>
     <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="17"/>
-      <c r="AK78" s="17"/>
+      <c r="AJ78" s="19"/>
+      <c r="AK78" s="19"/>
     </row>
     <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="17"/>
-      <c r="AK79" s="17"/>
+      <c r="AJ79" s="19"/>
+      <c r="AK79" s="19"/>
     </row>
     <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="17"/>
-      <c r="AK80" s="17"/>
+      <c r="AJ80" s="19"/>
+      <c r="AK80" s="19"/>
     </row>
     <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="17"/>
-      <c r="AK81" s="17"/>
+      <c r="AJ81" s="19"/>
+      <c r="AK81" s="19"/>
     </row>
     <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="17"/>
-      <c r="AK82" s="17"/>
+      <c r="AJ82" s="19"/>
+      <c r="AK82" s="19"/>
     </row>
     <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="17"/>
-      <c r="AK83" s="17"/>
+      <c r="AJ83" s="19"/>
+      <c r="AK83" s="19"/>
     </row>
     <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="17"/>
-      <c r="AK84" s="17"/>
+      <c r="AJ84" s="19"/>
+      <c r="AK84" s="19"/>
     </row>
     <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="17"/>
-      <c r="AK85" s="17"/>
+      <c r="AJ85" s="19"/>
+      <c r="AK85" s="19"/>
     </row>
     <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="17"/>
-      <c r="AK86" s="17"/>
+      <c r="AJ86" s="19"/>
+      <c r="AK86" s="19"/>
     </row>
     <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="17"/>
-      <c r="AK87" s="17"/>
+      <c r="AJ87" s="19"/>
+      <c r="AK87" s="19"/>
     </row>
     <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="17"/>
-      <c r="AK88" s="17"/>
+      <c r="AJ88" s="19"/>
+      <c r="AK88" s="19"/>
     </row>
     <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="17"/>
-      <c r="AK89" s="17"/>
+      <c r="AJ89" s="19"/>
+      <c r="AK89" s="19"/>
     </row>
     <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="17"/>
-      <c r="AK90" s="17"/>
+      <c r="AJ90" s="19"/>
+      <c r="AK90" s="19"/>
     </row>
     <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="17"/>
-      <c r="AK91" s="17"/>
+      <c r="AJ91" s="19"/>
+      <c r="AK91" s="19"/>
     </row>
     <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="17"/>
-      <c r="AK92" s="17"/>
+      <c r="AJ92" s="19"/>
+      <c r="AK92" s="19"/>
     </row>
     <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="17"/>
-      <c r="AK93" s="17"/>
+      <c r="AJ93" s="19"/>
+      <c r="AK93" s="19"/>
     </row>
     <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="17"/>
-      <c r="AK94" s="17"/>
+      <c r="AJ94" s="19"/>
+      <c r="AK94" s="19"/>
     </row>
     <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="17"/>
-      <c r="AK95" s="17"/>
+      <c r="AJ95" s="19"/>
+      <c r="AK95" s="19"/>
     </row>
     <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="17"/>
-      <c r="AK96" s="17"/>
+      <c r="AJ96" s="19"/>
+      <c r="AK96" s="19"/>
     </row>
     <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="17"/>
-      <c r="AK97" s="17"/>
+      <c r="AJ97" s="19"/>
+      <c r="AK97" s="19"/>
     </row>
     <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="17"/>
-      <c r="AK98" s="17"/>
+      <c r="AJ98" s="19"/>
+      <c r="AK98" s="19"/>
     </row>
     <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="17"/>
-      <c r="AK99" s="17"/>
+      <c r="AJ99" s="19"/>
+      <c r="AK99" s="19"/>
     </row>
     <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="17"/>
-      <c r="AK100" s="17"/>
+      <c r="AJ100" s="19"/>
+      <c r="AK100" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2260,26 +2329,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e9c3904391dfdb572e7cb9fb22afd49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9197d42b690c6e28e7629505631f20d" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -2514,10 +2563,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2534,20 +2614,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
-    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Move keywords to new page
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C6561-CE89-4229-942F-6AF62FF1B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E040549-92BB-4AEF-AD3D-AFFB95945F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="PIN Errors" sheetId="1" r:id="rId2"/>
     <sheet name="Other Errors" sheetId="3" r:id="rId3"/>
+    <sheet name="Assessable Key Words" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
   <si>
     <t># [LLINE]</t>
   </si>
@@ -272,12 +273,6 @@
     <t>"Yes" if the work description is missing. Empty otherwise.</t>
   </si>
   <si>
-    <t>"Yes" if the work description contains terms that indicate the permit is likely to be assessable. Empty otherwise.</t>
-  </si>
-  <si>
-    <t>Likely Assessable</t>
-  </si>
-  <si>
     <t>Column descriptions</t>
   </si>
   <si>
@@ -315,6 +310,15 @@
   </si>
   <si>
     <t>Permit rows with all other types of errors except for missing or invalid PINs.</t>
+  </si>
+  <si>
+    <t>Assessable Key Words</t>
+  </si>
+  <si>
+    <t>Comma separated list of matched keywords</t>
+  </si>
+  <si>
+    <t>List of key words which are matched with Notes [NOTE1] to identify likely assessable permits</t>
   </si>
 </sst>
 </file>
@@ -442,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -455,9 +459,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -476,6 +477,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,9 +500,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -535,9 +540,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,9 +575,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -605,9 +627,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -781,45 +820,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDD913F-9030-4CD4-850D-F7EAF1DE7A4C}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="137.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="137.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="15"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -827,12 +868,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -840,7 +881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,7 +889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -856,7 +897,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -864,7 +905,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -872,7 +913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -880,7 +921,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -888,7 +929,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -896,7 +937,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -904,7 +945,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -912,7 +953,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -920,7 +961,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -928,7 +969,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -936,7 +977,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -944,7 +985,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -952,7 +993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
@@ -960,7 +1001,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
@@ -968,7 +1009,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
@@ -976,7 +1017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -984,7 +1025,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -992,12 +1033,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>20</v>
       </c>
@@ -1005,7 +1046,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>21</v>
       </c>
@@ -1013,7 +1054,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
@@ -1021,7 +1062,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1070,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1078,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +1086,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -1053,7 +1094,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>27</v>
       </c>
@@ -1061,7 +1102,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1069,7 +1110,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1118,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>31</v>
       </c>
@@ -1093,7 +1134,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>32</v>
       </c>
@@ -1101,7 +1142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>33</v>
       </c>
@@ -1109,7 +1150,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>34</v>
       </c>
@@ -1117,77 +1158,92 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B50" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>79</v>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A53" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A53" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="14"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B60" t="s">
-        <v>92</v>
-      </c>
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="20"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1199,52 +1255,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AJ27" sqref="AJ27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.44140625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="52.85546875" style="12" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" customWidth="1"/>
+    <col min="35" max="35" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.88671875" style="11" customWidth="1"/>
+    <col min="37" max="37" width="20.33203125" style="11" customWidth="1"/>
+    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1305,456 +1361,456 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AI1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="18" t="s">
+      <c r="AK1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="19"/>
-      <c r="AK9" s="19"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="19"/>
-      <c r="AK10" s="19"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="19"/>
-      <c r="AK12" s="19"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="19"/>
-      <c r="AK13" s="19"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="19"/>
-      <c r="AK16" s="19"/>
-    </row>
-    <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-    </row>
-    <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="19"/>
-      <c r="AK18" s="19"/>
-    </row>
-    <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-    </row>
-    <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-    </row>
-    <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-    </row>
-    <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="19"/>
-      <c r="AK22" s="19"/>
-    </row>
-    <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="19"/>
-    </row>
-    <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="19"/>
-      <c r="AK24" s="19"/>
-    </row>
-    <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="19"/>
-      <c r="AK25" s="19"/>
-    </row>
-    <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="19"/>
-      <c r="AK26" s="19"/>
-    </row>
-    <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="19"/>
-      <c r="AK27" s="19"/>
-    </row>
-    <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="19"/>
-      <c r="AK28" s="19"/>
-    </row>
-    <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="19"/>
-      <c r="AK29" s="19"/>
-    </row>
-    <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="19"/>
-      <c r="AK30" s="19"/>
-    </row>
-    <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="19"/>
-      <c r="AK31" s="19"/>
-    </row>
-    <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="19"/>
-      <c r="AK32" s="19"/>
-    </row>
-    <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="19"/>
-      <c r="AK33" s="19"/>
-    </row>
-    <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="19"/>
-      <c r="AK34" s="19"/>
-    </row>
-    <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="19"/>
-      <c r="AK35" s="19"/>
-    </row>
-    <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="19"/>
-      <c r="AK36" s="19"/>
-    </row>
-    <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-    </row>
-    <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="19"/>
-      <c r="AK38" s="19"/>
-    </row>
-    <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="19"/>
-      <c r="AK39" s="19"/>
-    </row>
-    <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="19"/>
-      <c r="AK40" s="19"/>
-    </row>
-    <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="19"/>
-      <c r="AK41" s="19"/>
-    </row>
-    <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="19"/>
-      <c r="AK42" s="19"/>
-    </row>
-    <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="19"/>
-      <c r="AK43" s="19"/>
-    </row>
-    <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="19"/>
-      <c r="AK44" s="19"/>
-    </row>
-    <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="19"/>
-      <c r="AK45" s="19"/>
-    </row>
-    <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="19"/>
-      <c r="AK46" s="19"/>
-    </row>
-    <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="19"/>
-      <c r="AK47" s="19"/>
-    </row>
-    <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="19"/>
-      <c r="AK48" s="19"/>
-    </row>
-    <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="19"/>
-      <c r="AK49" s="19"/>
-    </row>
-    <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="19"/>
-      <c r="AK50" s="19"/>
-    </row>
-    <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="19"/>
-      <c r="AK51" s="19"/>
-    </row>
-    <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="19"/>
-      <c r="AK52" s="19"/>
-    </row>
-    <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="19"/>
-      <c r="AK53" s="19"/>
-    </row>
-    <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="19"/>
-      <c r="AK54" s="19"/>
-    </row>
-    <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="19"/>
-      <c r="AK55" s="19"/>
-    </row>
-    <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="19"/>
-      <c r="AK56" s="19"/>
-    </row>
-    <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="19"/>
-      <c r="AK57" s="19"/>
-    </row>
-    <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="19"/>
-      <c r="AK58" s="19"/>
-    </row>
-    <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="19"/>
-      <c r="AK59" s="19"/>
-    </row>
-    <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="19"/>
-      <c r="AK60" s="19"/>
-    </row>
-    <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="19"/>
-      <c r="AK61" s="19"/>
-    </row>
-    <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="19"/>
-      <c r="AK62" s="19"/>
-    </row>
-    <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="19"/>
-      <c r="AK63" s="19"/>
-    </row>
-    <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="19"/>
-      <c r="AK64" s="19"/>
-    </row>
-    <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="19"/>
-      <c r="AK65" s="19"/>
-    </row>
-    <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="19"/>
-      <c r="AK66" s="19"/>
-    </row>
-    <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="19"/>
-      <c r="AK67" s="19"/>
-    </row>
-    <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="19"/>
-      <c r="AK68" s="19"/>
-    </row>
-    <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="19"/>
-      <c r="AK69" s="19"/>
-    </row>
-    <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="19"/>
-      <c r="AK70" s="19"/>
-    </row>
-    <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="19"/>
-      <c r="AK71" s="19"/>
-    </row>
-    <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="19"/>
-      <c r="AK72" s="19"/>
-    </row>
-    <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="19"/>
-      <c r="AK73" s="19"/>
-    </row>
-    <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="19"/>
-      <c r="AK74" s="19"/>
-    </row>
-    <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="19"/>
-      <c r="AK75" s="19"/>
-    </row>
-    <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="19"/>
-      <c r="AK76" s="19"/>
-    </row>
-    <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="19"/>
-      <c r="AK77" s="19"/>
-    </row>
-    <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="19"/>
-      <c r="AK78" s="19"/>
-    </row>
-    <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="19"/>
-      <c r="AK79" s="19"/>
-    </row>
-    <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="19"/>
-      <c r="AK80" s="19"/>
-    </row>
-    <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="19"/>
-      <c r="AK81" s="19"/>
-    </row>
-    <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="19"/>
-      <c r="AK82" s="19"/>
-    </row>
-    <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="19"/>
-      <c r="AK83" s="19"/>
-    </row>
-    <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="19"/>
-      <c r="AK84" s="19"/>
-    </row>
-    <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="19"/>
-      <c r="AK85" s="19"/>
-    </row>
-    <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="19"/>
-      <c r="AK86" s="19"/>
-    </row>
-    <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="19"/>
-      <c r="AK87" s="19"/>
-    </row>
-    <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="19"/>
-      <c r="AK88" s="19"/>
-    </row>
-    <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="19"/>
-      <c r="AK89" s="19"/>
-    </row>
-    <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="19"/>
-      <c r="AK90" s="19"/>
-    </row>
-    <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="19"/>
-      <c r="AK91" s="19"/>
-    </row>
-    <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="19"/>
-      <c r="AK92" s="19"/>
-    </row>
-    <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="19"/>
-      <c r="AK93" s="19"/>
-    </row>
-    <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="19"/>
-      <c r="AK94" s="19"/>
-    </row>
-    <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="19"/>
-      <c r="AK95" s="19"/>
-    </row>
-    <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="19"/>
-      <c r="AK96" s="19"/>
-    </row>
-    <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="19"/>
-      <c r="AK97" s="19"/>
-    </row>
-    <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="19"/>
-      <c r="AK98" s="19"/>
-    </row>
-    <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="19"/>
-      <c r="AK99" s="19"/>
-    </row>
-    <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="19"/>
-      <c r="AK100" s="19"/>
+      <c r="AL1" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+    </row>
+    <row r="17" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+    </row>
+    <row r="18" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+    </row>
+    <row r="19" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+    </row>
+    <row r="20" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+    </row>
+    <row r="21" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+    </row>
+    <row r="22" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="18"/>
+    </row>
+    <row r="23" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="18"/>
+      <c r="AK23" s="18"/>
+    </row>
+    <row r="24" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ24" s="18"/>
+      <c r="AK24" s="18"/>
+    </row>
+    <row r="25" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+    </row>
+    <row r="26" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+    </row>
+    <row r="27" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+    </row>
+    <row r="28" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+    </row>
+    <row r="29" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+    </row>
+    <row r="30" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ30" s="18"/>
+      <c r="AK30" s="18"/>
+    </row>
+    <row r="31" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ31" s="18"/>
+      <c r="AK31" s="18"/>
+    </row>
+    <row r="32" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ32" s="18"/>
+      <c r="AK32" s="18"/>
+    </row>
+    <row r="33" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ33" s="18"/>
+      <c r="AK33" s="18"/>
+    </row>
+    <row r="34" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ34" s="18"/>
+      <c r="AK34" s="18"/>
+    </row>
+    <row r="35" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ35" s="18"/>
+      <c r="AK35" s="18"/>
+    </row>
+    <row r="36" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ36" s="18"/>
+      <c r="AK36" s="18"/>
+    </row>
+    <row r="37" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ37" s="18"/>
+      <c r="AK37" s="18"/>
+    </row>
+    <row r="38" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ38" s="18"/>
+      <c r="AK38" s="18"/>
+    </row>
+    <row r="39" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ39" s="18"/>
+      <c r="AK39" s="18"/>
+    </row>
+    <row r="40" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ40" s="18"/>
+      <c r="AK40" s="18"/>
+    </row>
+    <row r="41" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ41" s="18"/>
+      <c r="AK41" s="18"/>
+    </row>
+    <row r="42" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="18"/>
+    </row>
+    <row r="43" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ43" s="18"/>
+      <c r="AK43" s="18"/>
+    </row>
+    <row r="44" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ44" s="18"/>
+      <c r="AK44" s="18"/>
+    </row>
+    <row r="45" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ45" s="18"/>
+      <c r="AK45" s="18"/>
+    </row>
+    <row r="46" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ46" s="18"/>
+      <c r="AK46" s="18"/>
+    </row>
+    <row r="47" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ47" s="18"/>
+      <c r="AK47" s="18"/>
+    </row>
+    <row r="48" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ48" s="18"/>
+      <c r="AK48" s="18"/>
+    </row>
+    <row r="49" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ49" s="18"/>
+      <c r="AK49" s="18"/>
+    </row>
+    <row r="50" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ50" s="18"/>
+      <c r="AK50" s="18"/>
+    </row>
+    <row r="51" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ51" s="18"/>
+      <c r="AK51" s="18"/>
+    </row>
+    <row r="52" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ52" s="18"/>
+      <c r="AK52" s="18"/>
+    </row>
+    <row r="53" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ53" s="18"/>
+      <c r="AK53" s="18"/>
+    </row>
+    <row r="54" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ54" s="18"/>
+      <c r="AK54" s="18"/>
+    </row>
+    <row r="55" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ55" s="18"/>
+      <c r="AK55" s="18"/>
+    </row>
+    <row r="56" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ56" s="18"/>
+      <c r="AK56" s="18"/>
+    </row>
+    <row r="57" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ57" s="18"/>
+      <c r="AK57" s="18"/>
+    </row>
+    <row r="58" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ58" s="18"/>
+      <c r="AK58" s="18"/>
+    </row>
+    <row r="59" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ59" s="18"/>
+      <c r="AK59" s="18"/>
+    </row>
+    <row r="60" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ60" s="18"/>
+      <c r="AK60" s="18"/>
+    </row>
+    <row r="61" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ61" s="18"/>
+      <c r="AK61" s="18"/>
+    </row>
+    <row r="62" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ62" s="18"/>
+      <c r="AK62" s="18"/>
+    </row>
+    <row r="63" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ63" s="18"/>
+      <c r="AK63" s="18"/>
+    </row>
+    <row r="64" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ64" s="18"/>
+      <c r="AK64" s="18"/>
+    </row>
+    <row r="65" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ65" s="18"/>
+      <c r="AK65" s="18"/>
+    </row>
+    <row r="66" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ66" s="18"/>
+      <c r="AK66" s="18"/>
+    </row>
+    <row r="67" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ67" s="18"/>
+      <c r="AK67" s="18"/>
+    </row>
+    <row r="68" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ68" s="18"/>
+      <c r="AK68" s="18"/>
+    </row>
+    <row r="69" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ69" s="18"/>
+      <c r="AK69" s="18"/>
+    </row>
+    <row r="70" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ70" s="18"/>
+      <c r="AK70" s="18"/>
+    </row>
+    <row r="71" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ71" s="18"/>
+      <c r="AK71" s="18"/>
+    </row>
+    <row r="72" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ72" s="18"/>
+      <c r="AK72" s="18"/>
+    </row>
+    <row r="73" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ73" s="18"/>
+      <c r="AK73" s="18"/>
+    </row>
+    <row r="74" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ74" s="18"/>
+      <c r="AK74" s="18"/>
+    </row>
+    <row r="75" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ75" s="18"/>
+      <c r="AK75" s="18"/>
+    </row>
+    <row r="76" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ76" s="18"/>
+      <c r="AK76" s="18"/>
+    </row>
+    <row r="77" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ77" s="18"/>
+      <c r="AK77" s="18"/>
+    </row>
+    <row r="78" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ78" s="18"/>
+      <c r="AK78" s="18"/>
+    </row>
+    <row r="79" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ79" s="18"/>
+      <c r="AK79" s="18"/>
+    </row>
+    <row r="80" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ80" s="18"/>
+      <c r="AK80" s="18"/>
+    </row>
+    <row r="81" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ81" s="18"/>
+      <c r="AK81" s="18"/>
+    </row>
+    <row r="82" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ82" s="18"/>
+      <c r="AK82" s="18"/>
+    </row>
+    <row r="83" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ83" s="18"/>
+      <c r="AK83" s="18"/>
+    </row>
+    <row r="84" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ84" s="18"/>
+      <c r="AK84" s="18"/>
+    </row>
+    <row r="85" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ85" s="18"/>
+      <c r="AK85" s="18"/>
+    </row>
+    <row r="86" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ86" s="18"/>
+      <c r="AK86" s="18"/>
+    </row>
+    <row r="87" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ87" s="18"/>
+      <c r="AK87" s="18"/>
+    </row>
+    <row r="88" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ88" s="18"/>
+      <c r="AK88" s="18"/>
+    </row>
+    <row r="89" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ89" s="18"/>
+      <c r="AK89" s="18"/>
+    </row>
+    <row r="90" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ90" s="18"/>
+      <c r="AK90" s="18"/>
+    </row>
+    <row r="91" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ91" s="18"/>
+      <c r="AK91" s="18"/>
+    </row>
+    <row r="92" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ92" s="18"/>
+      <c r="AK92" s="18"/>
+    </row>
+    <row r="93" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ93" s="18"/>
+      <c r="AK93" s="18"/>
+    </row>
+    <row r="94" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ94" s="18"/>
+      <c r="AK94" s="18"/>
+    </row>
+    <row r="95" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ95" s="18"/>
+      <c r="AK95" s="18"/>
+    </row>
+    <row r="96" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ96" s="18"/>
+      <c r="AK96" s="18"/>
+    </row>
+    <row r="97" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ97" s="18"/>
+      <c r="AK97" s="18"/>
+    </row>
+    <row r="98" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ98" s="18"/>
+      <c r="AK98" s="18"/>
+    </row>
+    <row r="99" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ99" s="18"/>
+      <c r="AK99" s="18"/>
+    </row>
+    <row r="100" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ100" s="18"/>
+      <c r="AK100" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1766,52 +1822,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AN27" sqref="AN27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.44140625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="52.7109375" style="12" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" customWidth="1"/>
+    <col min="35" max="35" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.6640625" style="11" customWidth="1"/>
+    <col min="37" max="37" width="20.33203125" style="11" customWidth="1"/>
+    <col min="38" max="38" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1872,458 +1928,470 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AI1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="18" t="s">
+      <c r="AK1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="19"/>
-      <c r="AK9" s="19"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="19"/>
-      <c r="AK10" s="19"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="19"/>
-      <c r="AK12" s="19"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="19"/>
-      <c r="AK13" s="19"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="19"/>
-      <c r="AK16" s="19"/>
-    </row>
-    <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-    </row>
-    <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="19"/>
-      <c r="AK18" s="19"/>
-    </row>
-    <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-    </row>
-    <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-    </row>
-    <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-    </row>
-    <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="19"/>
-      <c r="AK22" s="19"/>
-    </row>
-    <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="19"/>
-    </row>
-    <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="19"/>
-      <c r="AK24" s="19"/>
-    </row>
-    <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="19"/>
-      <c r="AK25" s="19"/>
-    </row>
-    <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="19"/>
-      <c r="AK26" s="19"/>
-    </row>
-    <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="19"/>
-      <c r="AK27" s="19"/>
-    </row>
-    <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="19"/>
-      <c r="AK28" s="19"/>
-    </row>
-    <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="19"/>
-      <c r="AK29" s="19"/>
-    </row>
-    <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="19"/>
-      <c r="AK30" s="19"/>
-    </row>
-    <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="19"/>
-      <c r="AK31" s="19"/>
-    </row>
-    <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="19"/>
-      <c r="AK32" s="19"/>
-    </row>
-    <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="19"/>
-      <c r="AK33" s="19"/>
-    </row>
-    <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="19"/>
-      <c r="AK34" s="19"/>
-    </row>
-    <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="19"/>
-      <c r="AK35" s="19"/>
-    </row>
-    <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="19"/>
-      <c r="AK36" s="19"/>
-    </row>
-    <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-    </row>
-    <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="19"/>
-      <c r="AK38" s="19"/>
-    </row>
-    <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="19"/>
-      <c r="AK39" s="19"/>
-    </row>
-    <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="19"/>
-      <c r="AK40" s="19"/>
-    </row>
-    <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="19"/>
-      <c r="AK41" s="19"/>
-    </row>
-    <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="19"/>
-      <c r="AK42" s="19"/>
-    </row>
-    <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="19"/>
-      <c r="AK43" s="19"/>
-    </row>
-    <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="19"/>
-      <c r="AK44" s="19"/>
-    </row>
-    <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="19"/>
-      <c r="AK45" s="19"/>
-    </row>
-    <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="19"/>
-      <c r="AK46" s="19"/>
-    </row>
-    <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="19"/>
-      <c r="AK47" s="19"/>
-    </row>
-    <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="19"/>
-      <c r="AK48" s="19"/>
-    </row>
-    <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="19"/>
-      <c r="AK49" s="19"/>
-    </row>
-    <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="19"/>
-      <c r="AK50" s="19"/>
-    </row>
-    <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="19"/>
-      <c r="AK51" s="19"/>
-    </row>
-    <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="19"/>
-      <c r="AK52" s="19"/>
-    </row>
-    <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="19"/>
-      <c r="AK53" s="19"/>
-    </row>
-    <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="19"/>
-      <c r="AK54" s="19"/>
-    </row>
-    <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="19"/>
-      <c r="AK55" s="19"/>
-    </row>
-    <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="19"/>
-      <c r="AK56" s="19"/>
-    </row>
-    <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="19"/>
-      <c r="AK57" s="19"/>
-    </row>
-    <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="19"/>
-      <c r="AK58" s="19"/>
-    </row>
-    <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="19"/>
-      <c r="AK59" s="19"/>
-    </row>
-    <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="19"/>
-      <c r="AK60" s="19"/>
-    </row>
-    <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="19"/>
-      <c r="AK61" s="19"/>
-    </row>
-    <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="19"/>
-      <c r="AK62" s="19"/>
-    </row>
-    <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="19"/>
-      <c r="AK63" s="19"/>
-    </row>
-    <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="19"/>
-      <c r="AK64" s="19"/>
-    </row>
-    <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="19"/>
-      <c r="AK65" s="19"/>
-    </row>
-    <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="19"/>
-      <c r="AK66" s="19"/>
-    </row>
-    <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="19"/>
-      <c r="AK67" s="19"/>
-    </row>
-    <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="19"/>
-      <c r="AK68" s="19"/>
-    </row>
-    <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="19"/>
-      <c r="AK69" s="19"/>
-    </row>
-    <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="19"/>
-      <c r="AK70" s="19"/>
-    </row>
-    <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="19"/>
-      <c r="AK71" s="19"/>
-    </row>
-    <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="19"/>
-      <c r="AK72" s="19"/>
-    </row>
-    <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="19"/>
-      <c r="AK73" s="19"/>
-    </row>
-    <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="19"/>
-      <c r="AK74" s="19"/>
-    </row>
-    <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="19"/>
-      <c r="AK75" s="19"/>
-    </row>
-    <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="19"/>
-      <c r="AK76" s="19"/>
-    </row>
-    <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="19"/>
-      <c r="AK77" s="19"/>
-    </row>
-    <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="19"/>
-      <c r="AK78" s="19"/>
-    </row>
-    <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="19"/>
-      <c r="AK79" s="19"/>
-    </row>
-    <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="19"/>
-      <c r="AK80" s="19"/>
-    </row>
-    <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="19"/>
-      <c r="AK81" s="19"/>
-    </row>
-    <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="19"/>
-      <c r="AK82" s="19"/>
-    </row>
-    <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="19"/>
-      <c r="AK83" s="19"/>
-    </row>
-    <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="19"/>
-      <c r="AK84" s="19"/>
-    </row>
-    <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="19"/>
-      <c r="AK85" s="19"/>
-    </row>
-    <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="19"/>
-      <c r="AK86" s="19"/>
-    </row>
-    <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="19"/>
-      <c r="AK87" s="19"/>
-    </row>
-    <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="19"/>
-      <c r="AK88" s="19"/>
-    </row>
-    <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="19"/>
-      <c r="AK89" s="19"/>
-    </row>
-    <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="19"/>
-      <c r="AK90" s="19"/>
-    </row>
-    <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="19"/>
-      <c r="AK91" s="19"/>
-    </row>
-    <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="19"/>
-      <c r="AK92" s="19"/>
-    </row>
-    <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="19"/>
-      <c r="AK93" s="19"/>
-    </row>
-    <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="19"/>
-      <c r="AK94" s="19"/>
-    </row>
-    <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="19"/>
-      <c r="AK95" s="19"/>
-    </row>
-    <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="19"/>
-      <c r="AK96" s="19"/>
-    </row>
-    <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="19"/>
-      <c r="AK97" s="19"/>
-    </row>
-    <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="19"/>
-      <c r="AK98" s="19"/>
-    </row>
-    <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="19"/>
-      <c r="AK99" s="19"/>
-    </row>
-    <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="19"/>
-      <c r="AK100" s="19"/>
+      <c r="AL1" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+    </row>
+    <row r="17" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+    </row>
+    <row r="18" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+    </row>
+    <row r="19" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+    </row>
+    <row r="20" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+    </row>
+    <row r="21" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+    </row>
+    <row r="22" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="18"/>
+    </row>
+    <row r="23" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="18"/>
+      <c r="AK23" s="18"/>
+    </row>
+    <row r="24" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ24" s="18"/>
+      <c r="AK24" s="18"/>
+    </row>
+    <row r="25" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+    </row>
+    <row r="26" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+    </row>
+    <row r="27" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+    </row>
+    <row r="28" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+    </row>
+    <row r="29" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+    </row>
+    <row r="30" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ30" s="18"/>
+      <c r="AK30" s="18"/>
+    </row>
+    <row r="31" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ31" s="18"/>
+      <c r="AK31" s="18"/>
+    </row>
+    <row r="32" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ32" s="18"/>
+      <c r="AK32" s="18"/>
+    </row>
+    <row r="33" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ33" s="18"/>
+      <c r="AK33" s="18"/>
+    </row>
+    <row r="34" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ34" s="18"/>
+      <c r="AK34" s="18"/>
+    </row>
+    <row r="35" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ35" s="18"/>
+      <c r="AK35" s="18"/>
+    </row>
+    <row r="36" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ36" s="18"/>
+      <c r="AK36" s="18"/>
+    </row>
+    <row r="37" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ37" s="18"/>
+      <c r="AK37" s="18"/>
+    </row>
+    <row r="38" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ38" s="18"/>
+      <c r="AK38" s="18"/>
+    </row>
+    <row r="39" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ39" s="18"/>
+      <c r="AK39" s="18"/>
+    </row>
+    <row r="40" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ40" s="18"/>
+      <c r="AK40" s="18"/>
+    </row>
+    <row r="41" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ41" s="18"/>
+      <c r="AK41" s="18"/>
+    </row>
+    <row r="42" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="18"/>
+    </row>
+    <row r="43" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ43" s="18"/>
+      <c r="AK43" s="18"/>
+    </row>
+    <row r="44" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ44" s="18"/>
+      <c r="AK44" s="18"/>
+    </row>
+    <row r="45" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ45" s="18"/>
+      <c r="AK45" s="18"/>
+    </row>
+    <row r="46" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ46" s="18"/>
+      <c r="AK46" s="18"/>
+    </row>
+    <row r="47" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ47" s="18"/>
+      <c r="AK47" s="18"/>
+    </row>
+    <row r="48" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ48" s="18"/>
+      <c r="AK48" s="18"/>
+    </row>
+    <row r="49" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ49" s="18"/>
+      <c r="AK49" s="18"/>
+    </row>
+    <row r="50" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ50" s="18"/>
+      <c r="AK50" s="18"/>
+    </row>
+    <row r="51" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ51" s="18"/>
+      <c r="AK51" s="18"/>
+    </row>
+    <row r="52" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ52" s="18"/>
+      <c r="AK52" s="18"/>
+    </row>
+    <row r="53" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ53" s="18"/>
+      <c r="AK53" s="18"/>
+    </row>
+    <row r="54" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ54" s="18"/>
+      <c r="AK54" s="18"/>
+    </row>
+    <row r="55" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ55" s="18"/>
+      <c r="AK55" s="18"/>
+    </row>
+    <row r="56" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ56" s="18"/>
+      <c r="AK56" s="18"/>
+    </row>
+    <row r="57" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ57" s="18"/>
+      <c r="AK57" s="18"/>
+    </row>
+    <row r="58" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ58" s="18"/>
+      <c r="AK58" s="18"/>
+    </row>
+    <row r="59" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ59" s="18"/>
+      <c r="AK59" s="18"/>
+    </row>
+    <row r="60" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ60" s="18"/>
+      <c r="AK60" s="18"/>
+    </row>
+    <row r="61" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ61" s="18"/>
+      <c r="AK61" s="18"/>
+    </row>
+    <row r="62" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ62" s="18"/>
+      <c r="AK62" s="18"/>
+    </row>
+    <row r="63" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ63" s="18"/>
+      <c r="AK63" s="18"/>
+    </row>
+    <row r="64" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ64" s="18"/>
+      <c r="AK64" s="18"/>
+    </row>
+    <row r="65" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ65" s="18"/>
+      <c r="AK65" s="18"/>
+    </row>
+    <row r="66" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ66" s="18"/>
+      <c r="AK66" s="18"/>
+    </row>
+    <row r="67" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ67" s="18"/>
+      <c r="AK67" s="18"/>
+    </row>
+    <row r="68" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ68" s="18"/>
+      <c r="AK68" s="18"/>
+    </row>
+    <row r="69" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ69" s="18"/>
+      <c r="AK69" s="18"/>
+    </row>
+    <row r="70" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ70" s="18"/>
+      <c r="AK70" s="18"/>
+    </row>
+    <row r="71" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ71" s="18"/>
+      <c r="AK71" s="18"/>
+    </row>
+    <row r="72" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ72" s="18"/>
+      <c r="AK72" s="18"/>
+    </row>
+    <row r="73" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ73" s="18"/>
+      <c r="AK73" s="18"/>
+    </row>
+    <row r="74" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ74" s="18"/>
+      <c r="AK74" s="18"/>
+    </row>
+    <row r="75" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ75" s="18"/>
+      <c r="AK75" s="18"/>
+    </row>
+    <row r="76" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ76" s="18"/>
+      <c r="AK76" s="18"/>
+    </row>
+    <row r="77" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ77" s="18"/>
+      <c r="AK77" s="18"/>
+    </row>
+    <row r="78" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ78" s="18"/>
+      <c r="AK78" s="18"/>
+    </row>
+    <row r="79" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ79" s="18"/>
+      <c r="AK79" s="18"/>
+    </row>
+    <row r="80" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ80" s="18"/>
+      <c r="AK80" s="18"/>
+    </row>
+    <row r="81" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ81" s="18"/>
+      <c r="AK81" s="18"/>
+    </row>
+    <row r="82" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ82" s="18"/>
+      <c r="AK82" s="18"/>
+    </row>
+    <row r="83" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ83" s="18"/>
+      <c r="AK83" s="18"/>
+    </row>
+    <row r="84" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ84" s="18"/>
+      <c r="AK84" s="18"/>
+    </row>
+    <row r="85" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ85" s="18"/>
+      <c r="AK85" s="18"/>
+    </row>
+    <row r="86" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ86" s="18"/>
+      <c r="AK86" s="18"/>
+    </row>
+    <row r="87" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ87" s="18"/>
+      <c r="AK87" s="18"/>
+    </row>
+    <row r="88" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ88" s="18"/>
+      <c r="AK88" s="18"/>
+    </row>
+    <row r="89" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ89" s="18"/>
+      <c r="AK89" s="18"/>
+    </row>
+    <row r="90" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ90" s="18"/>
+      <c r="AK90" s="18"/>
+    </row>
+    <row r="91" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ91" s="18"/>
+      <c r="AK91" s="18"/>
+    </row>
+    <row r="92" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ92" s="18"/>
+      <c r="AK92" s="18"/>
+    </row>
+    <row r="93" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ93" s="18"/>
+      <c r="AK93" s="18"/>
+    </row>
+    <row r="94" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ94" s="18"/>
+      <c r="AK94" s="18"/>
+    </row>
+    <row r="95" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ95" s="18"/>
+      <c r="AK95" s="18"/>
+    </row>
+    <row r="96" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ96" s="18"/>
+      <c r="AK96" s="18"/>
+    </row>
+    <row r="97" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ97" s="18"/>
+      <c r="AK97" s="18"/>
+    </row>
+    <row r="98" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ98" s="18"/>
+      <c r="AK98" s="18"/>
+    </row>
+    <row r="99" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ99" s="18"/>
+      <c r="AK99" s="18"/>
+    </row>
+    <row r="100" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ100" s="18"/>
+      <c r="AK100" s="18"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE73ABCC-CEDD-4F2C-A825-3E1BD1092E34}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
move keywords out of function
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E040549-92BB-4AEF-AD3D-AFFB95945F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C960789E-62BB-4893-A45F-E5768C0FCF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="98">
   <si>
     <t># [LLINE]</t>
   </si>
@@ -319,6 +319,18 @@
   </si>
   <si>
     <t>List of key words which are matched with Notes [NOTE1] to identify likely assessable permits</t>
+  </si>
+  <si>
+    <t>Matched Keywords</t>
+  </si>
+  <si>
+    <t>List of Keywords</t>
+  </si>
+  <si>
+    <t>Modifying this table will not affect matches in other sheets.</t>
+  </si>
+  <si>
+    <t>Matched_Keywords</t>
   </si>
 </sst>
 </file>
@@ -822,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDD913F-9030-4CD4-850D-F7EAF1DE7A4C}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,7 +1193,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
         <v>92</v>
@@ -1257,7 +1269,7 @@
   <sheetViews>
     <sheetView topLeftCell="AJ1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ27" sqref="AJ27"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1413,7 +1425,7 @@
         <v>59</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -1822,9 +1834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN27" sqref="AN27"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1864,7 +1876,7 @@
     <col min="35" max="35" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="52.6640625" style="11" customWidth="1"/>
     <col min="37" max="37" width="20.33203125" style="11" customWidth="1"/>
-    <col min="38" max="38" width="18.88671875" customWidth="1"/>
+    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1980,7 +1992,7 @@
         <v>59</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -2378,25 +2390,61 @@
     <row r="100" spans="36:37" x14ac:dyDescent="0.3">
       <c r="AJ100" s="18"/>
       <c r="AK100" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE73ABCC-CEDD-4F2C-A825-3E1BD1092E34}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE73ABCC-CEDD-4F2C-A825-3E1BD1092E34}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e9c3904391dfdb572e7cb9fb22afd49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9197d42b690c6e28e7629505631f20d" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -2631,27 +2679,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D5D59B-9A62-4F83-956D-C544A82E46C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2668,23 +2715,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D5D59B-9A62-4F83-956D-C544A82E46C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
-    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tiny change to template
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C960789E-62BB-4893-A45F-E5768C0FCF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61AEB57-BF07-4F01-92DE-4832C29D5A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -327,10 +327,30 @@
     <t>List of Keywords</t>
   </si>
   <si>
-    <t>Modifying this table will not affect matches in other sheets.</t>
-  </si>
-  <si>
     <t>Matched_Keywords</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modifying this table will not affect matches in other sheets.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -458,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -493,6 +513,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1425,7 +1446,7 @@
         <v>59</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -1834,7 +1855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
@@ -1992,7 +2013,7 @@
         <v>59</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -2401,50 +2422,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE73ABCC-CEDD-4F2C-A825-3E1BD1092E34}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e9c3904391dfdb572e7cb9fb22afd49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9197d42b690c6e28e7629505631f20d" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -2679,10 +2681,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2699,20 +2732,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
-    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update with PR comments
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61AEB57-BF07-4F01-92DE-4832C29D5A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA175962-C4B9-49E8-BA5B-4D4D6B42FEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t># [LLINE]</t>
   </si>
@@ -315,9 +315,6 @@
     <t>Assessable Key Words</t>
   </si>
   <si>
-    <t>Comma separated list of matched keywords</t>
-  </si>
-  <si>
     <t>List of key words which are matched with Notes [NOTE1] to identify likely assessable permits</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
   </si>
   <si>
     <t>List of Keywords</t>
-  </si>
-  <si>
-    <t>Matched_Keywords</t>
   </si>
   <si>
     <r>
@@ -351,6 +345,9 @@
       </rPr>
       <t>Modifying this table will not affect matches in other sheets.</t>
     </r>
+  </si>
+  <si>
+    <t>Comma separated list of words in the Notes [NOTE1] field that match assessable keywords defined in the "Assessable Key Words" tab</t>
   </si>
 </sst>
 </file>
@@ -855,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDD913F-9030-4CD4-850D-F7EAF1DE7A4C}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,10 +1211,10 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.4">
@@ -1268,7 +1265,7 @@
         <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1288,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
@@ -1446,7 +1443,7 @@
         <v>59</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -2013,7 +2010,7 @@
         <v>59</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
@@ -2422,7 +2419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE73ABCC-CEDD-4F2C-A825-3E1BD1092E34}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2434,10 +2431,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
         <v>95</v>
-      </c>
-      <c r="B1" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23 update permits needing review sheet with new list of likely assessable keywords (#24)
* Move keywords to new page

* Working except for @ symbol

* Working for 1 row

* Revert to working

* Include string removals for excel

* Revert to original

* Working except for double keywords

* move keywords out of function

* tiny change to template

* Update permit_cleaning.py

* Update permit_cleaning.py

* Update permit_cleaning.py

* Update permit_cleaning.py

* lintr

* update with PR comments

* Remove build

* lintr
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C6561-CE89-4229-942F-6AF62FF1B659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA175962-C4B9-49E8-BA5B-4D4D6B42FEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="PIN Errors" sheetId="1" r:id="rId2"/>
     <sheet name="Other Errors" sheetId="3" r:id="rId3"/>
+    <sheet name="Assessable Key Words" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t># [LLINE]</t>
   </si>
@@ -272,12 +273,6 @@
     <t>"Yes" if the work description is missing. Empty otherwise.</t>
   </si>
   <si>
-    <t>"Yes" if the work description contains terms that indicate the permit is likely to be assessable. Empty otherwise.</t>
-  </si>
-  <si>
-    <t>Likely Assessable</t>
-  </si>
-  <si>
     <t>Column descriptions</t>
   </si>
   <si>
@@ -315,6 +310,44 @@
   </si>
   <si>
     <t>Permit rows with all other types of errors except for missing or invalid PINs.</t>
+  </si>
+  <si>
+    <t>Assessable Key Words</t>
+  </si>
+  <si>
+    <t>List of key words which are matched with Notes [NOTE1] to identify likely assessable permits</t>
+  </si>
+  <si>
+    <t>Matched Keywords</t>
+  </si>
+  <si>
+    <t>List of Keywords</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modifying this table will not affect matches in other sheets.</t>
+    </r>
+  </si>
+  <si>
+    <t>Comma separated list of words in the Notes [NOTE1] field that match assessable keywords defined in the "Assessable Key Words" tab</t>
   </si>
 </sst>
 </file>
@@ -442,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -455,9 +488,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -476,6 +506,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,9 +530,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -535,9 +570,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,9 +605,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -605,9 +657,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -781,45 +850,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDD913F-9030-4CD4-850D-F7EAF1DE7A4C}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="137.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="137.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="15"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="14"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -827,12 +898,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -840,7 +911,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,7 +919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -856,7 +927,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -864,7 +935,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -872,7 +943,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -880,7 +951,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -888,7 +959,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -896,7 +967,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -904,7 +975,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
@@ -912,7 +983,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -920,7 +991,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -928,7 +999,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
@@ -936,7 +1007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -944,7 +1015,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -952,7 +1023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
@@ -960,7 +1031,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
@@ -968,7 +1039,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
@@ -976,7 +1047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -984,7 +1055,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -992,12 +1063,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>20</v>
       </c>
@@ -1005,7 +1076,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>21</v>
       </c>
@@ -1013,7 +1084,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
@@ -1021,7 +1092,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1100,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1108,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>25</v>
       </c>
@@ -1045,7 +1116,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -1053,7 +1124,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>27</v>
       </c>
@@ -1061,7 +1132,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1069,7 +1140,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1148,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>31</v>
       </c>
@@ -1093,7 +1164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>32</v>
       </c>
@@ -1101,7 +1172,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>33</v>
       </c>
@@ -1109,7 +1180,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>34</v>
       </c>
@@ -1117,77 +1188,92 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B50" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>79</v>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A53" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A53" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="14"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>82</v>
       </c>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>92</v>
       </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="20"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1199,52 +1285,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.44140625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="52.85546875" style="12" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" customWidth="1"/>
+    <col min="35" max="35" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.88671875" style="11" customWidth="1"/>
+    <col min="37" max="37" width="20.33203125" style="11" customWidth="1"/>
+    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1305,456 +1391,456 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AI1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="18" t="s">
+      <c r="AK1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="19"/>
-      <c r="AK9" s="19"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="19"/>
-      <c r="AK10" s="19"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="19"/>
-      <c r="AK12" s="19"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="19"/>
-      <c r="AK13" s="19"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="19"/>
-      <c r="AK16" s="19"/>
-    </row>
-    <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-    </row>
-    <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="19"/>
-      <c r="AK18" s="19"/>
-    </row>
-    <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-    </row>
-    <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-    </row>
-    <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-    </row>
-    <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="19"/>
-      <c r="AK22" s="19"/>
-    </row>
-    <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="19"/>
-    </row>
-    <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="19"/>
-      <c r="AK24" s="19"/>
-    </row>
-    <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="19"/>
-      <c r="AK25" s="19"/>
-    </row>
-    <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="19"/>
-      <c r="AK26" s="19"/>
-    </row>
-    <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="19"/>
-      <c r="AK27" s="19"/>
-    </row>
-    <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="19"/>
-      <c r="AK28" s="19"/>
-    </row>
-    <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="19"/>
-      <c r="AK29" s="19"/>
-    </row>
-    <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="19"/>
-      <c r="AK30" s="19"/>
-    </row>
-    <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="19"/>
-      <c r="AK31" s="19"/>
-    </row>
-    <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="19"/>
-      <c r="AK32" s="19"/>
-    </row>
-    <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="19"/>
-      <c r="AK33" s="19"/>
-    </row>
-    <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="19"/>
-      <c r="AK34" s="19"/>
-    </row>
-    <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="19"/>
-      <c r="AK35" s="19"/>
-    </row>
-    <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="19"/>
-      <c r="AK36" s="19"/>
-    </row>
-    <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-    </row>
-    <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="19"/>
-      <c r="AK38" s="19"/>
-    </row>
-    <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="19"/>
-      <c r="AK39" s="19"/>
-    </row>
-    <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="19"/>
-      <c r="AK40" s="19"/>
-    </row>
-    <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="19"/>
-      <c r="AK41" s="19"/>
-    </row>
-    <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="19"/>
-      <c r="AK42" s="19"/>
-    </row>
-    <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="19"/>
-      <c r="AK43" s="19"/>
-    </row>
-    <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="19"/>
-      <c r="AK44" s="19"/>
-    </row>
-    <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="19"/>
-      <c r="AK45" s="19"/>
-    </row>
-    <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="19"/>
-      <c r="AK46" s="19"/>
-    </row>
-    <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="19"/>
-      <c r="AK47" s="19"/>
-    </row>
-    <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="19"/>
-      <c r="AK48" s="19"/>
-    </row>
-    <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="19"/>
-      <c r="AK49" s="19"/>
-    </row>
-    <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="19"/>
-      <c r="AK50" s="19"/>
-    </row>
-    <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="19"/>
-      <c r="AK51" s="19"/>
-    </row>
-    <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="19"/>
-      <c r="AK52" s="19"/>
-    </row>
-    <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="19"/>
-      <c r="AK53" s="19"/>
-    </row>
-    <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="19"/>
-      <c r="AK54" s="19"/>
-    </row>
-    <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="19"/>
-      <c r="AK55" s="19"/>
-    </row>
-    <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="19"/>
-      <c r="AK56" s="19"/>
-    </row>
-    <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="19"/>
-      <c r="AK57" s="19"/>
-    </row>
-    <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="19"/>
-      <c r="AK58" s="19"/>
-    </row>
-    <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="19"/>
-      <c r="AK59" s="19"/>
-    </row>
-    <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="19"/>
-      <c r="AK60" s="19"/>
-    </row>
-    <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="19"/>
-      <c r="AK61" s="19"/>
-    </row>
-    <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="19"/>
-      <c r="AK62" s="19"/>
-    </row>
-    <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="19"/>
-      <c r="AK63" s="19"/>
-    </row>
-    <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="19"/>
-      <c r="AK64" s="19"/>
-    </row>
-    <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="19"/>
-      <c r="AK65" s="19"/>
-    </row>
-    <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="19"/>
-      <c r="AK66" s="19"/>
-    </row>
-    <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="19"/>
-      <c r="AK67" s="19"/>
-    </row>
-    <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="19"/>
-      <c r="AK68" s="19"/>
-    </row>
-    <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="19"/>
-      <c r="AK69" s="19"/>
-    </row>
-    <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="19"/>
-      <c r="AK70" s="19"/>
-    </row>
-    <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="19"/>
-      <c r="AK71" s="19"/>
-    </row>
-    <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="19"/>
-      <c r="AK72" s="19"/>
-    </row>
-    <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="19"/>
-      <c r="AK73" s="19"/>
-    </row>
-    <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="19"/>
-      <c r="AK74" s="19"/>
-    </row>
-    <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="19"/>
-      <c r="AK75" s="19"/>
-    </row>
-    <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="19"/>
-      <c r="AK76" s="19"/>
-    </row>
-    <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="19"/>
-      <c r="AK77" s="19"/>
-    </row>
-    <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="19"/>
-      <c r="AK78" s="19"/>
-    </row>
-    <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="19"/>
-      <c r="AK79" s="19"/>
-    </row>
-    <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="19"/>
-      <c r="AK80" s="19"/>
-    </row>
-    <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="19"/>
-      <c r="AK81" s="19"/>
-    </row>
-    <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="19"/>
-      <c r="AK82" s="19"/>
-    </row>
-    <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="19"/>
-      <c r="AK83" s="19"/>
-    </row>
-    <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="19"/>
-      <c r="AK84" s="19"/>
-    </row>
-    <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="19"/>
-      <c r="AK85" s="19"/>
-    </row>
-    <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="19"/>
-      <c r="AK86" s="19"/>
-    </row>
-    <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="19"/>
-      <c r="AK87" s="19"/>
-    </row>
-    <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="19"/>
-      <c r="AK88" s="19"/>
-    </row>
-    <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="19"/>
-      <c r="AK89" s="19"/>
-    </row>
-    <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="19"/>
-      <c r="AK90" s="19"/>
-    </row>
-    <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="19"/>
-      <c r="AK91" s="19"/>
-    </row>
-    <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="19"/>
-      <c r="AK92" s="19"/>
-    </row>
-    <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="19"/>
-      <c r="AK93" s="19"/>
-    </row>
-    <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="19"/>
-      <c r="AK94" s="19"/>
-    </row>
-    <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="19"/>
-      <c r="AK95" s="19"/>
-    </row>
-    <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="19"/>
-      <c r="AK96" s="19"/>
-    </row>
-    <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="19"/>
-      <c r="AK97" s="19"/>
-    </row>
-    <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="19"/>
-      <c r="AK98" s="19"/>
-    </row>
-    <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="19"/>
-      <c r="AK99" s="19"/>
-    </row>
-    <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="19"/>
-      <c r="AK100" s="19"/>
+      <c r="AL1" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+    </row>
+    <row r="17" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+    </row>
+    <row r="18" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+    </row>
+    <row r="19" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+    </row>
+    <row r="20" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+    </row>
+    <row r="21" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+    </row>
+    <row r="22" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="18"/>
+    </row>
+    <row r="23" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="18"/>
+      <c r="AK23" s="18"/>
+    </row>
+    <row r="24" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ24" s="18"/>
+      <c r="AK24" s="18"/>
+    </row>
+    <row r="25" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+    </row>
+    <row r="26" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+    </row>
+    <row r="27" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+    </row>
+    <row r="28" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+    </row>
+    <row r="29" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+    </row>
+    <row r="30" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ30" s="18"/>
+      <c r="AK30" s="18"/>
+    </row>
+    <row r="31" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ31" s="18"/>
+      <c r="AK31" s="18"/>
+    </row>
+    <row r="32" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ32" s="18"/>
+      <c r="AK32" s="18"/>
+    </row>
+    <row r="33" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ33" s="18"/>
+      <c r="AK33" s="18"/>
+    </row>
+    <row r="34" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ34" s="18"/>
+      <c r="AK34" s="18"/>
+    </row>
+    <row r="35" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ35" s="18"/>
+      <c r="AK35" s="18"/>
+    </row>
+    <row r="36" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ36" s="18"/>
+      <c r="AK36" s="18"/>
+    </row>
+    <row r="37" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ37" s="18"/>
+      <c r="AK37" s="18"/>
+    </row>
+    <row r="38" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ38" s="18"/>
+      <c r="AK38" s="18"/>
+    </row>
+    <row r="39" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ39" s="18"/>
+      <c r="AK39" s="18"/>
+    </row>
+    <row r="40" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ40" s="18"/>
+      <c r="AK40" s="18"/>
+    </row>
+    <row r="41" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ41" s="18"/>
+      <c r="AK41" s="18"/>
+    </row>
+    <row r="42" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="18"/>
+    </row>
+    <row r="43" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ43" s="18"/>
+      <c r="AK43" s="18"/>
+    </row>
+    <row r="44" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ44" s="18"/>
+      <c r="AK44" s="18"/>
+    </row>
+    <row r="45" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ45" s="18"/>
+      <c r="AK45" s="18"/>
+    </row>
+    <row r="46" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ46" s="18"/>
+      <c r="AK46" s="18"/>
+    </row>
+    <row r="47" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ47" s="18"/>
+      <c r="AK47" s="18"/>
+    </row>
+    <row r="48" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ48" s="18"/>
+      <c r="AK48" s="18"/>
+    </row>
+    <row r="49" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ49" s="18"/>
+      <c r="AK49" s="18"/>
+    </row>
+    <row r="50" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ50" s="18"/>
+      <c r="AK50" s="18"/>
+    </row>
+    <row r="51" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ51" s="18"/>
+      <c r="AK51" s="18"/>
+    </row>
+    <row r="52" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ52" s="18"/>
+      <c r="AK52" s="18"/>
+    </row>
+    <row r="53" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ53" s="18"/>
+      <c r="AK53" s="18"/>
+    </row>
+    <row r="54" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ54" s="18"/>
+      <c r="AK54" s="18"/>
+    </row>
+    <row r="55" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ55" s="18"/>
+      <c r="AK55" s="18"/>
+    </row>
+    <row r="56" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ56" s="18"/>
+      <c r="AK56" s="18"/>
+    </row>
+    <row r="57" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ57" s="18"/>
+      <c r="AK57" s="18"/>
+    </row>
+    <row r="58" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ58" s="18"/>
+      <c r="AK58" s="18"/>
+    </row>
+    <row r="59" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ59" s="18"/>
+      <c r="AK59" s="18"/>
+    </row>
+    <row r="60" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ60" s="18"/>
+      <c r="AK60" s="18"/>
+    </row>
+    <row r="61" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ61" s="18"/>
+      <c r="AK61" s="18"/>
+    </row>
+    <row r="62" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ62" s="18"/>
+      <c r="AK62" s="18"/>
+    </row>
+    <row r="63" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ63" s="18"/>
+      <c r="AK63" s="18"/>
+    </row>
+    <row r="64" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ64" s="18"/>
+      <c r="AK64" s="18"/>
+    </row>
+    <row r="65" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ65" s="18"/>
+      <c r="AK65" s="18"/>
+    </row>
+    <row r="66" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ66" s="18"/>
+      <c r="AK66" s="18"/>
+    </row>
+    <row r="67" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ67" s="18"/>
+      <c r="AK67" s="18"/>
+    </row>
+    <row r="68" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ68" s="18"/>
+      <c r="AK68" s="18"/>
+    </row>
+    <row r="69" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ69" s="18"/>
+      <c r="AK69" s="18"/>
+    </row>
+    <row r="70" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ70" s="18"/>
+      <c r="AK70" s="18"/>
+    </row>
+    <row r="71" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ71" s="18"/>
+      <c r="AK71" s="18"/>
+    </row>
+    <row r="72" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ72" s="18"/>
+      <c r="AK72" s="18"/>
+    </row>
+    <row r="73" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ73" s="18"/>
+      <c r="AK73" s="18"/>
+    </row>
+    <row r="74" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ74" s="18"/>
+      <c r="AK74" s="18"/>
+    </row>
+    <row r="75" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ75" s="18"/>
+      <c r="AK75" s="18"/>
+    </row>
+    <row r="76" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ76" s="18"/>
+      <c r="AK76" s="18"/>
+    </row>
+    <row r="77" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ77" s="18"/>
+      <c r="AK77" s="18"/>
+    </row>
+    <row r="78" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ78" s="18"/>
+      <c r="AK78" s="18"/>
+    </row>
+    <row r="79" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ79" s="18"/>
+      <c r="AK79" s="18"/>
+    </row>
+    <row r="80" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ80" s="18"/>
+      <c r="AK80" s="18"/>
+    </row>
+    <row r="81" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ81" s="18"/>
+      <c r="AK81" s="18"/>
+    </row>
+    <row r="82" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ82" s="18"/>
+      <c r="AK82" s="18"/>
+    </row>
+    <row r="83" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ83" s="18"/>
+      <c r="AK83" s="18"/>
+    </row>
+    <row r="84" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ84" s="18"/>
+      <c r="AK84" s="18"/>
+    </row>
+    <row r="85" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ85" s="18"/>
+      <c r="AK85" s="18"/>
+    </row>
+    <row r="86" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ86" s="18"/>
+      <c r="AK86" s="18"/>
+    </row>
+    <row r="87" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ87" s="18"/>
+      <c r="AK87" s="18"/>
+    </row>
+    <row r="88" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ88" s="18"/>
+      <c r="AK88" s="18"/>
+    </row>
+    <row r="89" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ89" s="18"/>
+      <c r="AK89" s="18"/>
+    </row>
+    <row r="90" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ90" s="18"/>
+      <c r="AK90" s="18"/>
+    </row>
+    <row r="91" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ91" s="18"/>
+      <c r="AK91" s="18"/>
+    </row>
+    <row r="92" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ92" s="18"/>
+      <c r="AK92" s="18"/>
+    </row>
+    <row r="93" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ93" s="18"/>
+      <c r="AK93" s="18"/>
+    </row>
+    <row r="94" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ94" s="18"/>
+      <c r="AK94" s="18"/>
+    </row>
+    <row r="95" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ95" s="18"/>
+      <c r="AK95" s="18"/>
+    </row>
+    <row r="96" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ96" s="18"/>
+      <c r="AK96" s="18"/>
+    </row>
+    <row r="97" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ97" s="18"/>
+      <c r="AK97" s="18"/>
+    </row>
+    <row r="98" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ98" s="18"/>
+      <c r="AK98" s="18"/>
+    </row>
+    <row r="99" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ99" s="18"/>
+      <c r="AK99" s="18"/>
+    </row>
+    <row r="100" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ100" s="18"/>
+      <c r="AK100" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1766,52 +1852,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AL100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AL1" sqref="AL1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="53" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="122.42578125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="53" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="122.44140625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="109.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36.44140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="28" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="52.7109375" style="12" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" style="12" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" customWidth="1"/>
+    <col min="35" max="35" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="52.6640625" style="11" customWidth="1"/>
+    <col min="37" max="37" width="20.33203125" style="11" customWidth="1"/>
+    <col min="38" max="38" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1872,459 +1958,488 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="W1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AE1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AG1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AH1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AI1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="18" t="s">
+      <c r="AK1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="AL1" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="19"/>
-      <c r="AK6" s="19"/>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ7" s="19"/>
-      <c r="AK7" s="19"/>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ9" s="19"/>
-      <c r="AK9" s="19"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ10" s="19"/>
-      <c r="AK10" s="19"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ12" s="19"/>
-      <c r="AK12" s="19"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ13" s="19"/>
-      <c r="AK13" s="19"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ15" s="19"/>
-      <c r="AK15" s="19"/>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ16" s="19"/>
-      <c r="AK16" s="19"/>
-    </row>
-    <row r="17" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-    </row>
-    <row r="18" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ18" s="19"/>
-      <c r="AK18" s="19"/>
-    </row>
-    <row r="19" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-    </row>
-    <row r="20" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-    </row>
-    <row r="21" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-    </row>
-    <row r="22" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ22" s="19"/>
-      <c r="AK22" s="19"/>
-    </row>
-    <row r="23" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ23" s="19"/>
-      <c r="AK23" s="19"/>
-    </row>
-    <row r="24" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ24" s="19"/>
-      <c r="AK24" s="19"/>
-    </row>
-    <row r="25" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ25" s="19"/>
-      <c r="AK25" s="19"/>
-    </row>
-    <row r="26" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ26" s="19"/>
-      <c r="AK26" s="19"/>
-    </row>
-    <row r="27" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ27" s="19"/>
-      <c r="AK27" s="19"/>
-    </row>
-    <row r="28" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ28" s="19"/>
-      <c r="AK28" s="19"/>
-    </row>
-    <row r="29" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ29" s="19"/>
-      <c r="AK29" s="19"/>
-    </row>
-    <row r="30" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ30" s="19"/>
-      <c r="AK30" s="19"/>
-    </row>
-    <row r="31" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ31" s="19"/>
-      <c r="AK31" s="19"/>
-    </row>
-    <row r="32" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ32" s="19"/>
-      <c r="AK32" s="19"/>
-    </row>
-    <row r="33" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ33" s="19"/>
-      <c r="AK33" s="19"/>
-    </row>
-    <row r="34" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ34" s="19"/>
-      <c r="AK34" s="19"/>
-    </row>
-    <row r="35" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ35" s="19"/>
-      <c r="AK35" s="19"/>
-    </row>
-    <row r="36" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ36" s="19"/>
-      <c r="AK36" s="19"/>
-    </row>
-    <row r="37" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ37" s="19"/>
-      <c r="AK37" s="19"/>
-    </row>
-    <row r="38" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ38" s="19"/>
-      <c r="AK38" s="19"/>
-    </row>
-    <row r="39" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ39" s="19"/>
-      <c r="AK39" s="19"/>
-    </row>
-    <row r="40" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ40" s="19"/>
-      <c r="AK40" s="19"/>
-    </row>
-    <row r="41" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ41" s="19"/>
-      <c r="AK41" s="19"/>
-    </row>
-    <row r="42" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ42" s="19"/>
-      <c r="AK42" s="19"/>
-    </row>
-    <row r="43" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ43" s="19"/>
-      <c r="AK43" s="19"/>
-    </row>
-    <row r="44" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ44" s="19"/>
-      <c r="AK44" s="19"/>
-    </row>
-    <row r="45" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ45" s="19"/>
-      <c r="AK45" s="19"/>
-    </row>
-    <row r="46" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="19"/>
-      <c r="AK46" s="19"/>
-    </row>
-    <row r="47" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="19"/>
-      <c r="AK47" s="19"/>
-    </row>
-    <row r="48" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="19"/>
-      <c r="AK48" s="19"/>
-    </row>
-    <row r="49" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ49" s="19"/>
-      <c r="AK49" s="19"/>
-    </row>
-    <row r="50" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ50" s="19"/>
-      <c r="AK50" s="19"/>
-    </row>
-    <row r="51" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ51" s="19"/>
-      <c r="AK51" s="19"/>
-    </row>
-    <row r="52" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ52" s="19"/>
-      <c r="AK52" s="19"/>
-    </row>
-    <row r="53" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ53" s="19"/>
-      <c r="AK53" s="19"/>
-    </row>
-    <row r="54" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="19"/>
-      <c r="AK54" s="19"/>
-    </row>
-    <row r="55" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="19"/>
-      <c r="AK55" s="19"/>
-    </row>
-    <row r="56" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="19"/>
-      <c r="AK56" s="19"/>
-    </row>
-    <row r="57" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="19"/>
-      <c r="AK57" s="19"/>
-    </row>
-    <row r="58" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ58" s="19"/>
-      <c r="AK58" s="19"/>
-    </row>
-    <row r="59" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ59" s="19"/>
-      <c r="AK59" s="19"/>
-    </row>
-    <row r="60" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ60" s="19"/>
-      <c r="AK60" s="19"/>
-    </row>
-    <row r="61" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ61" s="19"/>
-      <c r="AK61" s="19"/>
-    </row>
-    <row r="62" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ62" s="19"/>
-      <c r="AK62" s="19"/>
-    </row>
-    <row r="63" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ63" s="19"/>
-      <c r="AK63" s="19"/>
-    </row>
-    <row r="64" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ64" s="19"/>
-      <c r="AK64" s="19"/>
-    </row>
-    <row r="65" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ65" s="19"/>
-      <c r="AK65" s="19"/>
-    </row>
-    <row r="66" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ66" s="19"/>
-      <c r="AK66" s="19"/>
-    </row>
-    <row r="67" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ67" s="19"/>
-      <c r="AK67" s="19"/>
-    </row>
-    <row r="68" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ68" s="19"/>
-      <c r="AK68" s="19"/>
-    </row>
-    <row r="69" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ69" s="19"/>
-      <c r="AK69" s="19"/>
-    </row>
-    <row r="70" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ70" s="19"/>
-      <c r="AK70" s="19"/>
-    </row>
-    <row r="71" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ71" s="19"/>
-      <c r="AK71" s="19"/>
-    </row>
-    <row r="72" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ72" s="19"/>
-      <c r="AK72" s="19"/>
-    </row>
-    <row r="73" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ73" s="19"/>
-      <c r="AK73" s="19"/>
-    </row>
-    <row r="74" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ74" s="19"/>
-      <c r="AK74" s="19"/>
-    </row>
-    <row r="75" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ75" s="19"/>
-      <c r="AK75" s="19"/>
-    </row>
-    <row r="76" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ76" s="19"/>
-      <c r="AK76" s="19"/>
-    </row>
-    <row r="77" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ77" s="19"/>
-      <c r="AK77" s="19"/>
-    </row>
-    <row r="78" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ78" s="19"/>
-      <c r="AK78" s="19"/>
-    </row>
-    <row r="79" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ79" s="19"/>
-      <c r="AK79" s="19"/>
-    </row>
-    <row r="80" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ80" s="19"/>
-      <c r="AK80" s="19"/>
-    </row>
-    <row r="81" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ81" s="19"/>
-      <c r="AK81" s="19"/>
-    </row>
-    <row r="82" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ82" s="19"/>
-      <c r="AK82" s="19"/>
-    </row>
-    <row r="83" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ83" s="19"/>
-      <c r="AK83" s="19"/>
-    </row>
-    <row r="84" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ84" s="19"/>
-      <c r="AK84" s="19"/>
-    </row>
-    <row r="85" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ85" s="19"/>
-      <c r="AK85" s="19"/>
-    </row>
-    <row r="86" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="19"/>
-      <c r="AK86" s="19"/>
-    </row>
-    <row r="87" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ87" s="19"/>
-      <c r="AK87" s="19"/>
-    </row>
-    <row r="88" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ88" s="19"/>
-      <c r="AK88" s="19"/>
-    </row>
-    <row r="89" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ89" s="19"/>
-      <c r="AK89" s="19"/>
-    </row>
-    <row r="90" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ90" s="19"/>
-      <c r="AK90" s="19"/>
-    </row>
-    <row r="91" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="19"/>
-      <c r="AK91" s="19"/>
-    </row>
-    <row r="92" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ92" s="19"/>
-      <c r="AK92" s="19"/>
-    </row>
-    <row r="93" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ93" s="19"/>
-      <c r="AK93" s="19"/>
-    </row>
-    <row r="94" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ94" s="19"/>
-      <c r="AK94" s="19"/>
-    </row>
-    <row r="95" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ95" s="19"/>
-      <c r="AK95" s="19"/>
-    </row>
-    <row r="96" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ96" s="19"/>
-      <c r="AK96" s="19"/>
-    </row>
-    <row r="97" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ97" s="19"/>
-      <c r="AK97" s="19"/>
-    </row>
-    <row r="98" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ98" s="19"/>
-      <c r="AK98" s="19"/>
-    </row>
-    <row r="99" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ99" s="19"/>
-      <c r="AK99" s="19"/>
-    </row>
-    <row r="100" spans="36:37" x14ac:dyDescent="0.25">
-      <c r="AJ100" s="19"/>
-      <c r="AK100" s="19"/>
+      <c r="AL1" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+    </row>
+    <row r="17" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+    </row>
+    <row r="18" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+    </row>
+    <row r="19" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+    </row>
+    <row r="20" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+    </row>
+    <row r="21" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+    </row>
+    <row r="22" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="18"/>
+    </row>
+    <row r="23" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ23" s="18"/>
+      <c r="AK23" s="18"/>
+    </row>
+    <row r="24" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ24" s="18"/>
+      <c r="AK24" s="18"/>
+    </row>
+    <row r="25" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+    </row>
+    <row r="26" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+    </row>
+    <row r="27" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+    </row>
+    <row r="28" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+    </row>
+    <row r="29" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+    </row>
+    <row r="30" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ30" s="18"/>
+      <c r="AK30" s="18"/>
+    </row>
+    <row r="31" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ31" s="18"/>
+      <c r="AK31" s="18"/>
+    </row>
+    <row r="32" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ32" s="18"/>
+      <c r="AK32" s="18"/>
+    </row>
+    <row r="33" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ33" s="18"/>
+      <c r="AK33" s="18"/>
+    </row>
+    <row r="34" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ34" s="18"/>
+      <c r="AK34" s="18"/>
+    </row>
+    <row r="35" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ35" s="18"/>
+      <c r="AK35" s="18"/>
+    </row>
+    <row r="36" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ36" s="18"/>
+      <c r="AK36" s="18"/>
+    </row>
+    <row r="37" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ37" s="18"/>
+      <c r="AK37" s="18"/>
+    </row>
+    <row r="38" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ38" s="18"/>
+      <c r="AK38" s="18"/>
+    </row>
+    <row r="39" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ39" s="18"/>
+      <c r="AK39" s="18"/>
+    </row>
+    <row r="40" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ40" s="18"/>
+      <c r="AK40" s="18"/>
+    </row>
+    <row r="41" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ41" s="18"/>
+      <c r="AK41" s="18"/>
+    </row>
+    <row r="42" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="18"/>
+    </row>
+    <row r="43" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ43" s="18"/>
+      <c r="AK43" s="18"/>
+    </row>
+    <row r="44" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ44" s="18"/>
+      <c r="AK44" s="18"/>
+    </row>
+    <row r="45" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ45" s="18"/>
+      <c r="AK45" s="18"/>
+    </row>
+    <row r="46" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ46" s="18"/>
+      <c r="AK46" s="18"/>
+    </row>
+    <row r="47" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ47" s="18"/>
+      <c r="AK47" s="18"/>
+    </row>
+    <row r="48" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ48" s="18"/>
+      <c r="AK48" s="18"/>
+    </row>
+    <row r="49" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ49" s="18"/>
+      <c r="AK49" s="18"/>
+    </row>
+    <row r="50" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ50" s="18"/>
+      <c r="AK50" s="18"/>
+    </row>
+    <row r="51" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ51" s="18"/>
+      <c r="AK51" s="18"/>
+    </row>
+    <row r="52" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ52" s="18"/>
+      <c r="AK52" s="18"/>
+    </row>
+    <row r="53" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ53" s="18"/>
+      <c r="AK53" s="18"/>
+    </row>
+    <row r="54" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ54" s="18"/>
+      <c r="AK54" s="18"/>
+    </row>
+    <row r="55" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ55" s="18"/>
+      <c r="AK55" s="18"/>
+    </row>
+    <row r="56" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ56" s="18"/>
+      <c r="AK56" s="18"/>
+    </row>
+    <row r="57" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ57" s="18"/>
+      <c r="AK57" s="18"/>
+    </row>
+    <row r="58" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ58" s="18"/>
+      <c r="AK58" s="18"/>
+    </row>
+    <row r="59" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ59" s="18"/>
+      <c r="AK59" s="18"/>
+    </row>
+    <row r="60" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ60" s="18"/>
+      <c r="AK60" s="18"/>
+    </row>
+    <row r="61" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ61" s="18"/>
+      <c r="AK61" s="18"/>
+    </row>
+    <row r="62" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ62" s="18"/>
+      <c r="AK62" s="18"/>
+    </row>
+    <row r="63" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ63" s="18"/>
+      <c r="AK63" s="18"/>
+    </row>
+    <row r="64" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ64" s="18"/>
+      <c r="AK64" s="18"/>
+    </row>
+    <row r="65" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ65" s="18"/>
+      <c r="AK65" s="18"/>
+    </row>
+    <row r="66" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ66" s="18"/>
+      <c r="AK66" s="18"/>
+    </row>
+    <row r="67" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ67" s="18"/>
+      <c r="AK67" s="18"/>
+    </row>
+    <row r="68" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ68" s="18"/>
+      <c r="AK68" s="18"/>
+    </row>
+    <row r="69" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ69" s="18"/>
+      <c r="AK69" s="18"/>
+    </row>
+    <row r="70" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ70" s="18"/>
+      <c r="AK70" s="18"/>
+    </row>
+    <row r="71" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ71" s="18"/>
+      <c r="AK71" s="18"/>
+    </row>
+    <row r="72" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ72" s="18"/>
+      <c r="AK72" s="18"/>
+    </row>
+    <row r="73" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ73" s="18"/>
+      <c r="AK73" s="18"/>
+    </row>
+    <row r="74" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ74" s="18"/>
+      <c r="AK74" s="18"/>
+    </row>
+    <row r="75" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ75" s="18"/>
+      <c r="AK75" s="18"/>
+    </row>
+    <row r="76" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ76" s="18"/>
+      <c r="AK76" s="18"/>
+    </row>
+    <row r="77" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ77" s="18"/>
+      <c r="AK77" s="18"/>
+    </row>
+    <row r="78" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ78" s="18"/>
+      <c r="AK78" s="18"/>
+    </row>
+    <row r="79" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ79" s="18"/>
+      <c r="AK79" s="18"/>
+    </row>
+    <row r="80" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ80" s="18"/>
+      <c r="AK80" s="18"/>
+    </row>
+    <row r="81" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ81" s="18"/>
+      <c r="AK81" s="18"/>
+    </row>
+    <row r="82" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ82" s="18"/>
+      <c r="AK82" s="18"/>
+    </row>
+    <row r="83" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ83" s="18"/>
+      <c r="AK83" s="18"/>
+    </row>
+    <row r="84" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ84" s="18"/>
+      <c r="AK84" s="18"/>
+    </row>
+    <row r="85" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ85" s="18"/>
+      <c r="AK85" s="18"/>
+    </row>
+    <row r="86" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ86" s="18"/>
+      <c r="AK86" s="18"/>
+    </row>
+    <row r="87" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ87" s="18"/>
+      <c r="AK87" s="18"/>
+    </row>
+    <row r="88" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ88" s="18"/>
+      <c r="AK88" s="18"/>
+    </row>
+    <row r="89" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ89" s="18"/>
+      <c r="AK89" s="18"/>
+    </row>
+    <row r="90" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ90" s="18"/>
+      <c r="AK90" s="18"/>
+    </row>
+    <row r="91" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ91" s="18"/>
+      <c r="AK91" s="18"/>
+    </row>
+    <row r="92" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ92" s="18"/>
+      <c r="AK92" s="18"/>
+    </row>
+    <row r="93" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ93" s="18"/>
+      <c r="AK93" s="18"/>
+    </row>
+    <row r="94" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ94" s="18"/>
+      <c r="AK94" s="18"/>
+    </row>
+    <row r="95" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ95" s="18"/>
+      <c r="AK95" s="18"/>
+    </row>
+    <row r="96" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ96" s="18"/>
+      <c r="AK96" s="18"/>
+    </row>
+    <row r="97" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ97" s="18"/>
+      <c r="AK97" s="18"/>
+    </row>
+    <row r="98" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ98" s="18"/>
+      <c r="AK98" s="18"/>
+    </row>
+    <row r="99" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ99" s="18"/>
+      <c r="AK99" s="18"/>
+    </row>
+    <row r="100" spans="36:37" x14ac:dyDescent="0.3">
+      <c r="AJ100" s="18"/>
+      <c r="AK100" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE73ABCC-CEDD-4F2C-A825-3E1BD1092E34}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
make it work on all sheets
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00D4E89-4DA2-4A16-A127-27E11C56D11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F29536-1279-4B29-8FCC-63807C0E639C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Assessable Key Words" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -906,7 +907,7 @@
   <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1338,6 @@
       <c r="B64" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="cVikwc6f8l5lDrtiFgmjt2SnpQDJJAkVRfBDQzSiTeClxh72ulx9RoqU6Jcgm2/tLz3bgwv/mTzX58YWDJvT1Q==" saltValue="Nxh3YTxBoq+jNPo9eGTWHw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1349,7 +1349,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,7 +1928,6 @@
       <c r="AK100" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rxgEFnSZvCTUcQqLOlE12zGJIMvT9z7gqe5sXn+jcBV70eRqiu9R086W4hnursYQYZbdLfb8pvWcAfJ7yBC9BQ==" saltValue="qTOEz4o+mngFL5wVTVAvwg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1940,7 +1939,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,7 +2517,6 @@
       <c r="AK100" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dGsGFBC0QN4/RwVTHRYnxBjqz8UTJBLvpwupFc55LQ11TCvBFBhL70gMchf6QkMng6LrXSd2n8A0oBToxwNzZg==" saltValue="zHnXizz0CReB+yS+/zfSpw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -2529,7 +2527,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2547,13 +2545,32 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Z9jf+T6pbtHdrlDSlVFxCAyXrrOyNCLanrRll7pgLAhMAO6vr5SgsQItcuFY+Qxsc1ib3JmY1x7qErh4PiHm3A==" saltValue="xOncBCS6M3dN4rTrKvcEdQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e9c3904391dfdb572e7cb9fb22afd49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9197d42b690c6e28e7629505631f20d" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -2788,27 +2805,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D5D59B-9A62-4F83-956D-C544A82E46C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2825,23 +2841,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D5D59B-9A62-4F83-956D-C544A82E46C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
-    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add row height fix
</commit_message>
<xml_diff>
--- a/chicago/templates/permits_needing_review.xlsx
+++ b/chicago/templates/permits_needing_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damajor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D90A8C-2C4E-4EB9-B087-C2350D295ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDE2A6E-9656-4859-8750-2F1F17413A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="5260" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-67320" yWindow="-5385" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -1046,9 +1046,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2307" sqref="C2307"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2284" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1057,7 @@
     <col min="2" max="2" width="11.5703125" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="109.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52.85546875" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="24" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="28" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" style="28" bestFit="1" customWidth="1"/>
@@ -1636,9 +1636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADE8290-BEBC-4760-ABEF-A71140CD6C10}">
   <dimension ref="A1:AM100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1646,7 @@
     <col min="1" max="1" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="10" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="28" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="10" bestFit="1" customWidth="1"/>
@@ -2250,26 +2250,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e9c3904391dfdb572e7cb9fb22afd49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c9197d42b690c6e28e7629505631f20d" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -2504,26 +2484,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D5D59B-9A62-4F83-956D-C544A82E46C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
-    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADA0474B-9F98-46F2-87E6-5AFDF174CFEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2540,4 +2521,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A916EAB6-040B-42FD-BC35-B17D273B5C97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37D5D59B-9A62-4F83-956D-C544A82E46C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>